<commit_message>
more sheet stats beig read
</commit_message>
<xml_diff>
--- a/RotoShootUnityProject/Assets/Resources/mySheet.xlsx
+++ b/RotoShootUnityProject/Assets/Resources/mySheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\UnityProjects\RotoShoot\RotoShootUnityProject\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2B8B97-E5E2-4BDB-AE0B-16BFAB4A6533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A82F1D20-6423-4497-8C51-B3DEFE6122F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37992" yWindow="-1560" windowWidth="33348" windowHeight="19944" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mySheet (4)" sheetId="4" r:id="rId1"/>
@@ -239,7 +239,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -431,6 +431,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -592,11 +604,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -956,7 +970,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B102" sqref="B102"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,7 +978,7 @@
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="20.5703125" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
     <col min="17" max="17" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -972,52 +986,52 @@
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="5" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tweaked the spinning mine behaviour. made the smartbomb work on spinningmine.
</commit_message>
<xml_diff>
--- a/RotoShootUnityProject/Assets/Resources/mySheet.xlsx
+++ b/RotoShootUnityProject/Assets/Resources/mySheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\UnityProjects\RotoShoot\RotoShootUnityProject\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211EEB43-C534-46BC-AF78-9A228DA2D5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD170AD-3158-47B5-BEB3-83FA615FD93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="90" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="37605" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mySheet (4)" sheetId="4" r:id="rId1"/>
@@ -1067,7 +1067,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O102" sqref="O102"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,10 +1142,10 @@
         <v>0.1</v>
       </c>
       <c r="C2" s="1">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="D2" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1">
         <v>5</v>
@@ -1193,23 +1193,23 @@
       </c>
       <c r="B3">
         <f>(B$2+((SUM($A3-1)/SUM($A$101-1))*(SUM(B$101-B$2))))</f>
-        <v>0.60404040404040404</v>
+        <v>0.40202020202020206</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:H18" si="0">(C$2+((SUM($A3-1)/SUM($A$101-1))*(SUM(C$101-C$2))))</f>
-        <v>0.19898989898989899</v>
+        <v>0.39797979797979799</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>1.9828282828282828</v>
+        <v>2.9737373737373738</v>
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>5.1515151515151514</v>
+        <v>5.1010101010101012</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
-        <v>10.1010101010101</v>
+        <v>10.05050505050505</v>
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
@@ -1234,7 +1234,7 @@
       </c>
       <c r="M3">
         <f t="shared" ref="M3:O66" si="2">(M$2+((SUM($A3-1)/SUM($A$101-1))*(SUM(M$101-M$2))))</f>
-        <v>2</v>
+        <v>1.7474747474747474</v>
       </c>
       <c r="N3">
         <v>-1</v>
@@ -1256,23 +1256,23 @@
       </c>
       <c r="B4">
         <f t="shared" ref="B4:B5" si="3">(B$2+((SUM($A4-1)/SUM($A$101-1))*(SUM(B$101-B$2))))</f>
-        <v>1.1080808080808082</v>
+        <v>0.70404040404040402</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>0.19797979797979798</v>
+        <v>0.39595959595959596</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>1.9656565656565657</v>
+        <v>2.9474747474747476</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>5.3030303030303028</v>
+        <v>5.2020202020202024</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>10.202020202020202</v>
+        <v>10.1010101010101</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
@@ -1297,7 +1297,7 @@
       </c>
       <c r="M4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2.4949494949494948</v>
       </c>
       <c r="N4">
         <v>-1</v>
@@ -1319,23 +1319,23 @@
       </c>
       <c r="B5">
         <f t="shared" si="3"/>
-        <v>1.6121212121212123</v>
+        <v>1.0060606060606061</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>0.19696969696969699</v>
+        <v>0.39393939393939398</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>1.9484848484848485</v>
+        <v>2.9212121212121214</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>5.454545454545455</v>
+        <v>5.3030303030303028</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>10.303030303030303</v>
+        <v>10.151515151515152</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
@@ -1360,7 +1360,7 @@
       </c>
       <c r="M5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3.2424242424242427</v>
       </c>
       <c r="N5">
         <v>-1</v>
@@ -1382,23 +1382,23 @@
       </c>
       <c r="B6">
         <f t="shared" ref="B6" si="4">(B$2+((SUM(A6-1)/SUM(A$101-1))*(SUM(B$101-B$2))))</f>
-        <v>2.1161616161616164</v>
+        <v>1.3080808080808082</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>0.19595959595959597</v>
+        <v>0.39191919191919194</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>1.9313131313131313</v>
+        <v>2.8949494949494952</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>5.6060606060606064</v>
+        <v>5.404040404040404</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>10.404040404040405</v>
+        <v>10.202020202020202</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
@@ -1423,7 +1423,7 @@
       </c>
       <c r="M6">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>3.9898989898989901</v>
       </c>
       <c r="N6">
         <v>-1</v>
@@ -1445,23 +1445,23 @@
       </c>
       <c r="B7">
         <f t="shared" ref="B7:B67" si="5">(B$2+((SUM(A7-1)/SUM(A$101-1))*(SUM(B$101-B$2))))</f>
-        <v>2.62020202020202</v>
+        <v>1.61010101010101</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>0.19494949494949496</v>
+        <v>0.38989898989898991</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>1.9141414141414141</v>
+        <v>2.8686868686868685</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>5.7575757575757578</v>
+        <v>5.5050505050505052</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>10.505050505050505</v>
+        <v>10.252525252525253</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="M7">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4.737373737373737</v>
       </c>
       <c r="N7">
         <v>-1</v>
@@ -1508,23 +1508,23 @@
       </c>
       <c r="B8">
         <f t="shared" si="5"/>
-        <v>3.1242424242424245</v>
+        <v>1.9121212121212121</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>0.19393939393939394</v>
+        <v>0.38787878787878788</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>1.896969696969697</v>
+        <v>2.8424242424242423</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>5.9090909090909092</v>
+        <v>5.6060606060606064</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>10.606060606060606</v>
+        <v>10.303030303030303</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
@@ -1549,7 +1549,7 @@
       </c>
       <c r="M8">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>5.4848484848484853</v>
       </c>
       <c r="N8">
         <v>-1</v>
@@ -1571,23 +1571,23 @@
       </c>
       <c r="B9">
         <f t="shared" si="5"/>
-        <v>3.6282828282828281</v>
+        <v>2.2141414141414142</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>0.19292929292929295</v>
+        <v>0.3858585858585859</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>1.8797979797979798</v>
+        <v>2.8161616161616161</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>6.0606060606060606</v>
+        <v>5.7070707070707067</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>10.707070707070708</v>
+        <v>10.353535353535353</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
@@ -1612,7 +1612,7 @@
       </c>
       <c r="M9">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>6.2323232323232318</v>
       </c>
       <c r="N9">
         <v>-1</v>
@@ -1634,23 +1634,23 @@
       </c>
       <c r="B10">
         <f t="shared" si="5"/>
-        <v>4.1323232323232322</v>
+        <v>2.5161616161616163</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>0.19191919191919193</v>
+        <v>0.38383838383838387</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>1.8626262626262626</v>
+        <v>2.7898989898989899</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>6.2121212121212119</v>
+        <v>5.808080808080808</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>10.808080808080808</v>
+        <v>10.404040404040405</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="M10">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>6.9797979797979801</v>
       </c>
       <c r="N10">
         <v>-1</v>
@@ -1697,23 +1697,23 @@
       </c>
       <c r="B11">
         <f t="shared" si="5"/>
-        <v>4.6363636363636358</v>
+        <v>2.8181818181818183</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>0.19090909090909092</v>
+        <v>0.38181818181818183</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>1.8454545454545455</v>
+        <v>2.7636363636363637</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>6.3636363636363633</v>
+        <v>5.9090909090909092</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>10.90909090909091</v>
+        <v>10.454545454545455</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
@@ -1738,7 +1738,7 @@
       </c>
       <c r="M11">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>7.7272727272727275</v>
       </c>
       <c r="N11">
         <v>-1</v>
@@ -1760,23 +1760,23 @@
       </c>
       <c r="B12">
         <f t="shared" si="5"/>
-        <v>5.1404040404040394</v>
+        <v>3.12020202020202</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>0.1898989898989899</v>
+        <v>0.3797979797979798</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>1.8282828282828283</v>
+        <v>2.7373737373737375</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>6.5151515151515156</v>
+        <v>6.0101010101010104</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>11.01010101010101</v>
+        <v>10.505050505050505</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
@@ -1801,7 +1801,7 @@
       </c>
       <c r="M12">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>8.474747474747474</v>
       </c>
       <c r="N12">
         <v>-1</v>
@@ -1823,23 +1823,23 @@
       </c>
       <c r="B13">
         <f t="shared" si="5"/>
-        <v>5.6444444444444439</v>
+        <v>3.4222222222222221</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>0.18888888888888891</v>
+        <v>0.37777777777777782</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>1.8111111111111111</v>
+        <v>2.7111111111111112</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>6.6666666666666661</v>
+        <v>6.1111111111111107</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>11.111111111111111</v>
+        <v>10.555555555555555</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
@@ -1864,7 +1864,7 @@
       </c>
       <c r="M13">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>9.2222222222222214</v>
       </c>
       <c r="N13">
         <v>-1</v>
@@ -1886,23 +1886,23 @@
       </c>
       <c r="B14">
         <f t="shared" si="5"/>
-        <v>6.1484848484848484</v>
+        <v>3.7242424242424241</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>0.1878787878787879</v>
+        <v>0.37575757575757579</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>1.7939393939393939</v>
+        <v>2.6848484848484846</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>6.8181818181818183</v>
+        <v>6.2121212121212119</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>11.212121212121213</v>
+        <v>10.606060606060606</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="M14">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>9.9696969696969706</v>
       </c>
       <c r="N14">
         <v>-1</v>
@@ -1949,23 +1949,23 @@
       </c>
       <c r="B15">
         <f t="shared" si="5"/>
-        <v>6.652525252525253</v>
+        <v>4.0262626262626267</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>0.18686868686868688</v>
+        <v>0.37373737373737376</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>1.7767676767676768</v>
+        <v>2.6585858585858584</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>6.9696969696969697</v>
+        <v>6.3131313131313131</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>11.313131313131313</v>
+        <v>10.656565656565657</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
@@ -1990,7 +1990,7 @@
       </c>
       <c r="M15">
         <f t="shared" si="2"/>
-        <v>14.000000000000002</v>
+        <v>10.717171717171718</v>
       </c>
       <c r="N15">
         <v>-1</v>
@@ -2012,23 +2012,23 @@
       </c>
       <c r="B16">
         <f t="shared" si="5"/>
-        <v>7.1565656565656557</v>
+        <v>4.3282828282828278</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>0.18585858585858586</v>
+        <v>0.37171717171717172</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>1.7595959595959596</v>
+        <v>2.6323232323232322</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>7.1212121212121211</v>
+        <v>6.4141414141414144</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>11.414141414141413</v>
+        <v>10.707070707070708</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
@@ -2053,7 +2053,7 @@
       </c>
       <c r="M16">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>11.464646464646464</v>
       </c>
       <c r="N16">
         <v>-1</v>
@@ -2075,23 +2075,23 @@
       </c>
       <c r="B17">
         <f t="shared" si="5"/>
-        <v>7.6606060606060602</v>
+        <v>4.6303030303030299</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>0.18484848484848487</v>
+        <v>0.36969696969696975</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>1.7424242424242424</v>
+        <v>2.606060606060606</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>7.2727272727272734</v>
+        <v>6.5151515151515156</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>11.515151515151516</v>
+        <v>10.757575757575758</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
@@ -2116,7 +2116,7 @@
       </c>
       <c r="M17">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>12.212121212121213</v>
       </c>
       <c r="N17">
         <v>-1</v>
@@ -2138,23 +2138,23 @@
       </c>
       <c r="B18">
         <f t="shared" si="5"/>
-        <v>8.1646464646464647</v>
+        <v>4.932323232323232</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>0.18383838383838386</v>
+        <v>0.36767676767676771</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>1.7252525252525253</v>
+        <v>2.5797979797979798</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>7.4242424242424239</v>
+        <v>6.6161616161616159</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>11.616161616161616</v>
+        <v>10.808080808080808</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="M18">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>12.95959595959596</v>
       </c>
       <c r="N18">
         <v>-1</v>
@@ -2201,23 +2201,23 @@
       </c>
       <c r="B19">
         <f t="shared" si="5"/>
-        <v>8.6686868686868674</v>
+        <v>5.2343434343434332</v>
       </c>
       <c r="C19">
         <f t="shared" ref="C19:D46" si="6">(C$2+((SUM($A19-1)/SUM($A$101-1))*(SUM(C$101-C$2))))</f>
-        <v>0.18282828282828284</v>
+        <v>0.36565656565656568</v>
       </c>
       <c r="D19">
         <f t="shared" si="6"/>
-        <v>1.7080808080808081</v>
+        <v>2.5535353535353535</v>
       </c>
       <c r="E19">
         <f t="shared" ref="E19:E82" si="7">(E$2+((SUM($A19-1)/SUM($A$101-1))*(SUM(E$101-E$2))))</f>
-        <v>7.5757575757575761</v>
+        <v>6.7171717171717171</v>
       </c>
       <c r="F19">
         <f t="shared" ref="F19:F82" si="8">(F$2+((SUM($A19-1)/SUM($A$101-1))*(SUM(F$101-F$2))))</f>
-        <v>11.717171717171716</v>
+        <v>10.858585858585858</v>
       </c>
       <c r="G19">
         <f t="shared" ref="G19:H82" si="9">(G$2+((SUM($A19-1)/SUM($A$101-1))*(SUM(G$101-G$2))))</f>
@@ -2242,7 +2242,7 @@
       </c>
       <c r="M19">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>13.707070707070706</v>
       </c>
       <c r="N19">
         <v>-1</v>
@@ -2264,23 +2264,23 @@
       </c>
       <c r="B20">
         <f t="shared" si="5"/>
-        <v>9.172727272727272</v>
+        <v>5.5363636363636362</v>
       </c>
       <c r="C20">
         <f t="shared" si="6"/>
-        <v>0.18181818181818182</v>
+        <v>0.36363636363636365</v>
       </c>
       <c r="D20">
         <f t="shared" si="6"/>
-        <v>1.6909090909090909</v>
+        <v>2.5272727272727273</v>
       </c>
       <c r="E20">
         <f t="shared" si="7"/>
-        <v>7.7272727272727275</v>
+        <v>6.8181818181818183</v>
       </c>
       <c r="F20">
         <f t="shared" si="8"/>
-        <v>11.818181818181818</v>
+        <v>10.90909090909091</v>
       </c>
       <c r="G20">
         <f t="shared" si="9"/>
@@ -2305,7 +2305,7 @@
       </c>
       <c r="M20">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>14.454545454545455</v>
       </c>
       <c r="N20">
         <v>-1</v>
@@ -2327,23 +2327,23 @@
       </c>
       <c r="B21">
         <f t="shared" si="5"/>
-        <v>9.6767676767676747</v>
+        <v>5.8383838383838373</v>
       </c>
       <c r="C21">
         <f t="shared" si="6"/>
-        <v>0.18080808080808081</v>
+        <v>0.36161616161616161</v>
       </c>
       <c r="D21">
         <f t="shared" si="6"/>
-        <v>1.6737373737373737</v>
+        <v>2.5010101010101011</v>
       </c>
       <c r="E21">
         <f t="shared" si="7"/>
-        <v>7.8787878787878789</v>
+        <v>6.9191919191919187</v>
       </c>
       <c r="F21">
         <f t="shared" si="8"/>
-        <v>11.919191919191919</v>
+        <v>10.95959595959596</v>
       </c>
       <c r="G21">
         <f t="shared" si="9"/>
@@ -2368,7 +2368,7 @@
       </c>
       <c r="M21">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>15.202020202020201</v>
       </c>
       <c r="N21">
         <v>-1</v>
@@ -2390,23 +2390,23 @@
       </c>
       <c r="B22">
         <f t="shared" si="5"/>
-        <v>10.180808080808079</v>
+        <v>6.1404040404040394</v>
       </c>
       <c r="C22">
         <f t="shared" si="6"/>
-        <v>0.17979797979797982</v>
+        <v>0.35959595959595964</v>
       </c>
       <c r="D22">
         <f t="shared" si="6"/>
-        <v>1.6565656565656566</v>
+        <v>2.4747474747474749</v>
       </c>
       <c r="E22">
         <f t="shared" si="7"/>
-        <v>8.0303030303030312</v>
+        <v>7.0202020202020208</v>
       </c>
       <c r="F22">
         <f t="shared" si="8"/>
-        <v>12.020202020202021</v>
+        <v>11.01010101010101</v>
       </c>
       <c r="G22">
         <f t="shared" si="9"/>
@@ -2431,7 +2431,7 @@
       </c>
       <c r="M22">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>15.94949494949495</v>
       </c>
       <c r="N22">
         <v>-1</v>
@@ -2453,23 +2453,23 @@
       </c>
       <c r="B23">
         <f t="shared" si="5"/>
-        <v>10.684848484848484</v>
+        <v>6.4424242424242424</v>
       </c>
       <c r="C23">
         <f t="shared" si="6"/>
-        <v>0.1787878787878788</v>
+        <v>0.3575757575757576</v>
       </c>
       <c r="D23">
         <f t="shared" si="6"/>
-        <v>1.6393939393939394</v>
+        <v>2.4484848484848483</v>
       </c>
       <c r="E23">
         <f t="shared" si="7"/>
-        <v>8.1818181818181817</v>
+        <v>7.1212121212121211</v>
       </c>
       <c r="F23">
         <f t="shared" si="8"/>
-        <v>12.121212121212121</v>
+        <v>11.060606060606061</v>
       </c>
       <c r="G23">
         <f t="shared" si="9"/>
@@ -2494,7 +2494,7 @@
       </c>
       <c r="M23">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>16.696969696969695</v>
       </c>
       <c r="N23">
         <v>-1</v>
@@ -2516,23 +2516,23 @@
       </c>
       <c r="B24">
         <f t="shared" si="5"/>
-        <v>11.188888888888888</v>
+        <v>6.7444444444444436</v>
       </c>
       <c r="C24">
         <f t="shared" si="6"/>
-        <v>0.17777777777777778</v>
+        <v>0.35555555555555557</v>
       </c>
       <c r="D24">
         <f t="shared" si="6"/>
-        <v>1.6222222222222222</v>
+        <v>2.4222222222222225</v>
       </c>
       <c r="E24">
         <f t="shared" si="7"/>
-        <v>8.3333333333333321</v>
+        <v>7.2222222222222223</v>
       </c>
       <c r="F24">
         <f t="shared" si="8"/>
-        <v>12.222222222222221</v>
+        <v>11.111111111111111</v>
       </c>
       <c r="G24">
         <f t="shared" si="9"/>
@@ -2557,7 +2557,7 @@
       </c>
       <c r="M24">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>17.444444444444443</v>
       </c>
       <c r="N24">
         <v>-1</v>
@@ -2579,23 +2579,23 @@
       </c>
       <c r="B25">
         <f t="shared" si="5"/>
-        <v>11.692929292929293</v>
+        <v>7.0464646464646457</v>
       </c>
       <c r="C25">
         <f t="shared" si="6"/>
-        <v>0.17676767676767677</v>
+        <v>0.35353535353535354</v>
       </c>
       <c r="D25">
         <f t="shared" si="6"/>
-        <v>1.6050505050505051</v>
+        <v>2.3959595959595958</v>
       </c>
       <c r="E25">
         <f t="shared" si="7"/>
-        <v>8.4848484848484844</v>
+        <v>7.3232323232323235</v>
       </c>
       <c r="F25">
         <f t="shared" si="8"/>
-        <v>12.323232323232324</v>
+        <v>11.161616161616161</v>
       </c>
       <c r="G25">
         <f t="shared" si="9"/>
@@ -2620,7 +2620,7 @@
       </c>
       <c r="M25">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>18.19191919191919</v>
       </c>
       <c r="N25">
         <v>-1</v>
@@ -2642,23 +2642,23 @@
       </c>
       <c r="B26">
         <f t="shared" si="5"/>
-        <v>12.196969696969697</v>
+        <v>7.3484848484848477</v>
       </c>
       <c r="C26">
         <f t="shared" si="6"/>
-        <v>0.17575757575757578</v>
+        <v>0.35151515151515156</v>
       </c>
       <c r="D26">
         <f t="shared" si="6"/>
-        <v>1.5878787878787879</v>
+        <v>2.3696969696969696</v>
       </c>
       <c r="E26">
         <f t="shared" si="7"/>
-        <v>8.6363636363636367</v>
+        <v>7.4242424242424239</v>
       </c>
       <c r="F26">
         <f t="shared" si="8"/>
-        <v>12.424242424242424</v>
+        <v>11.212121212121213</v>
       </c>
       <c r="G26">
         <f t="shared" si="9"/>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="M26">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>18.939393939393941</v>
       </c>
       <c r="N26">
         <v>-1</v>
@@ -2705,23 +2705,23 @@
       </c>
       <c r="B27">
         <f t="shared" si="5"/>
-        <v>12.701010101010102</v>
+        <v>7.6505050505050507</v>
       </c>
       <c r="C27">
         <f t="shared" si="6"/>
-        <v>0.17474747474747476</v>
+        <v>0.34949494949494953</v>
       </c>
       <c r="D27">
         <f t="shared" si="6"/>
-        <v>1.5707070707070707</v>
+        <v>2.3434343434343434</v>
       </c>
       <c r="E27">
         <f t="shared" si="7"/>
-        <v>8.787878787878789</v>
+        <v>7.525252525252526</v>
       </c>
       <c r="F27">
         <f t="shared" si="8"/>
-        <v>12.525252525252526</v>
+        <v>11.262626262626263</v>
       </c>
       <c r="G27">
         <f t="shared" si="9"/>
@@ -2746,7 +2746,7 @@
       </c>
       <c r="M27">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>19.686868686868689</v>
       </c>
       <c r="N27">
         <v>-1</v>
@@ -2768,23 +2768,23 @@
       </c>
       <c r="B28">
         <f t="shared" si="5"/>
-        <v>13.205050505050506</v>
+        <v>7.9525252525252528</v>
       </c>
       <c r="C28">
         <f t="shared" si="6"/>
-        <v>0.17373737373737375</v>
+        <v>0.34747474747474749</v>
       </c>
       <c r="D28">
         <f t="shared" si="6"/>
-        <v>1.5535353535353535</v>
+        <v>2.3171717171717172</v>
       </c>
       <c r="E28">
         <f t="shared" si="7"/>
-        <v>8.9393939393939394</v>
+        <v>7.6262626262626263</v>
       </c>
       <c r="F28">
         <f t="shared" si="8"/>
-        <v>12.626262626262626</v>
+        <v>11.313131313131313</v>
       </c>
       <c r="G28">
         <f t="shared" si="9"/>
@@ -2809,7 +2809,7 @@
       </c>
       <c r="M28">
         <f t="shared" si="2"/>
-        <v>27.000000000000004</v>
+        <v>20.434343434343436</v>
       </c>
       <c r="N28">
         <v>-1</v>
@@ -2831,23 +2831,23 @@
       </c>
       <c r="B29">
         <f t="shared" si="5"/>
-        <v>13.709090909090907</v>
+        <v>8.254545454545454</v>
       </c>
       <c r="C29">
         <f t="shared" si="6"/>
-        <v>0.17272727272727273</v>
+        <v>0.34545454545454546</v>
       </c>
       <c r="D29">
         <f t="shared" si="6"/>
-        <v>1.5363636363636364</v>
+        <v>2.290909090909091</v>
       </c>
       <c r="E29">
         <f t="shared" si="7"/>
-        <v>9.0909090909090899</v>
+        <v>7.7272727272727266</v>
       </c>
       <c r="F29">
         <f t="shared" si="8"/>
-        <v>12.727272727272727</v>
+        <v>11.363636363636363</v>
       </c>
       <c r="G29">
         <f t="shared" si="9"/>
@@ -2872,7 +2872,7 @@
       </c>
       <c r="M29">
         <f t="shared" si="2"/>
-        <v>27.999999999999996</v>
+        <v>21.18181818181818</v>
       </c>
       <c r="N29">
         <v>-1</v>
@@ -2894,23 +2894,23 @@
       </c>
       <c r="B30">
         <f t="shared" si="5"/>
-        <v>14.213131313131312</v>
+        <v>8.556565656565656</v>
       </c>
       <c r="C30">
         <f t="shared" si="6"/>
-        <v>0.17171717171717171</v>
+        <v>0.34343434343434343</v>
       </c>
       <c r="D30">
         <f t="shared" si="6"/>
-        <v>1.5191919191919192</v>
+        <v>2.2646464646464648</v>
       </c>
       <c r="E30">
         <f t="shared" si="7"/>
-        <v>9.2424242424242422</v>
+        <v>7.8282828282828287</v>
       </c>
       <c r="F30">
         <f t="shared" si="8"/>
-        <v>12.828282828282829</v>
+        <v>11.414141414141413</v>
       </c>
       <c r="G30">
         <f t="shared" si="9"/>
@@ -2935,7 +2935,7 @@
       </c>
       <c r="M30">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>21.929292929292927</v>
       </c>
       <c r="N30">
         <v>-1</v>
@@ -2957,23 +2957,23 @@
       </c>
       <c r="B31">
         <f t="shared" si="5"/>
-        <v>14.717171717171716</v>
+        <v>8.8585858585858581</v>
       </c>
       <c r="C31">
         <f t="shared" si="6"/>
-        <v>0.17070707070707072</v>
+        <v>0.34141414141414145</v>
       </c>
       <c r="D31">
         <f t="shared" si="6"/>
-        <v>1.502020202020202</v>
+        <v>2.2383838383838386</v>
       </c>
       <c r="E31">
         <f t="shared" si="7"/>
-        <v>9.3939393939393945</v>
+        <v>7.9292929292929291</v>
       </c>
       <c r="F31">
         <f t="shared" si="8"/>
-        <v>12.929292929292929</v>
+        <v>11.464646464646464</v>
       </c>
       <c r="G31">
         <f t="shared" si="9"/>
@@ -2998,7 +2998,7 @@
       </c>
       <c r="M31">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>22.676767676767678</v>
       </c>
       <c r="N31">
         <v>-1</v>
@@ -3020,23 +3020,23 @@
       </c>
       <c r="B32">
         <f t="shared" si="5"/>
-        <v>15.221212121212121</v>
+        <v>9.1606060606060602</v>
       </c>
       <c r="C32">
         <f t="shared" si="6"/>
-        <v>0.16969696969696971</v>
+        <v>0.33939393939393941</v>
       </c>
       <c r="D32">
         <f t="shared" si="6"/>
-        <v>1.4848484848484849</v>
+        <v>2.2121212121212119</v>
       </c>
       <c r="E32">
         <f t="shared" si="7"/>
-        <v>9.5454545454545467</v>
+        <v>8.0303030303030312</v>
       </c>
       <c r="F32">
         <f t="shared" si="8"/>
-        <v>13.030303030303031</v>
+        <v>11.515151515151516</v>
       </c>
       <c r="G32">
         <f t="shared" si="9"/>
@@ -3061,7 +3061,7 @@
       </c>
       <c r="M32">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>23.424242424242426</v>
       </c>
       <c r="N32">
         <v>-1</v>
@@ -3083,23 +3083,23 @@
       </c>
       <c r="B33">
         <f t="shared" si="5"/>
-        <v>15.725252525252525</v>
+        <v>9.4626262626262623</v>
       </c>
       <c r="C33">
         <f t="shared" si="6"/>
-        <v>0.16868686868686869</v>
+        <v>0.33737373737373738</v>
       </c>
       <c r="D33">
         <f t="shared" si="6"/>
-        <v>1.4676767676767677</v>
+        <v>2.1858585858585857</v>
       </c>
       <c r="E33">
         <f t="shared" si="7"/>
-        <v>9.6969696969696972</v>
+        <v>8.1313131313131315</v>
       </c>
       <c r="F33">
         <f t="shared" si="8"/>
-        <v>13.131313131313131</v>
+        <v>11.565656565656566</v>
       </c>
       <c r="G33">
         <f t="shared" si="9"/>
@@ -3124,7 +3124,7 @@
       </c>
       <c r="M33">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>24.171717171717173</v>
       </c>
       <c r="N33">
         <v>-1</v>
@@ -3146,23 +3146,23 @@
       </c>
       <c r="B34">
         <f t="shared" si="5"/>
-        <v>16.229292929292932</v>
+        <v>9.7646464646464644</v>
       </c>
       <c r="C34">
         <f t="shared" si="6"/>
-        <v>0.16767676767676767</v>
+        <v>0.33535353535353535</v>
       </c>
       <c r="D34">
         <f t="shared" si="6"/>
-        <v>1.4505050505050505</v>
+        <v>2.1595959595959595</v>
       </c>
       <c r="E34">
         <f t="shared" si="7"/>
-        <v>9.8484848484848477</v>
+        <v>8.2323232323232318</v>
       </c>
       <c r="F34">
         <f t="shared" si="8"/>
-        <v>13.232323232323232</v>
+        <v>11.616161616161616</v>
       </c>
       <c r="G34">
         <f t="shared" si="9"/>
@@ -3187,7 +3187,7 @@
       </c>
       <c r="M34">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>24.91919191919192</v>
       </c>
       <c r="N34">
         <v>-1</v>
@@ -3209,23 +3209,23 @@
       </c>
       <c r="B35">
         <f t="shared" si="5"/>
-        <v>16.733333333333334</v>
+        <v>10.066666666666665</v>
       </c>
       <c r="C35">
         <f t="shared" si="6"/>
-        <v>0.16666666666666669</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="D35">
         <f t="shared" si="6"/>
-        <v>1.4333333333333333</v>
+        <v>2.1333333333333333</v>
       </c>
       <c r="E35">
         <f t="shared" si="7"/>
-        <v>10</v>
+        <v>8.3333333333333321</v>
       </c>
       <c r="F35">
         <f t="shared" si="8"/>
-        <v>13.333333333333332</v>
+        <v>11.666666666666666</v>
       </c>
       <c r="G35">
         <f t="shared" si="9"/>
@@ -3250,7 +3250,7 @@
       </c>
       <c r="M35">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>25.666666666666664</v>
       </c>
       <c r="N35">
         <v>-1</v>
@@ -3272,23 +3272,23 @@
       </c>
       <c r="B36">
         <f t="shared" si="5"/>
-        <v>17.237373737373737</v>
+        <v>10.368686868686867</v>
       </c>
       <c r="C36">
         <f t="shared" si="6"/>
-        <v>0.16565656565656567</v>
+        <v>0.33131313131313134</v>
       </c>
       <c r="D36">
         <f t="shared" si="6"/>
-        <v>1.4161616161616162</v>
+        <v>2.1070707070707071</v>
       </c>
       <c r="E36">
         <f t="shared" si="7"/>
-        <v>10.151515151515152</v>
+        <v>8.4343434343434343</v>
       </c>
       <c r="F36">
         <f t="shared" si="8"/>
-        <v>13.434343434343434</v>
+        <v>11.717171717171716</v>
       </c>
       <c r="G36">
         <f t="shared" si="9"/>
@@ -3313,7 +3313,7 @@
       </c>
       <c r="M36">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>26.414141414141412</v>
       </c>
       <c r="N36">
         <v>-1</v>
@@ -3335,23 +3335,23 @@
       </c>
       <c r="B37">
         <f t="shared" si="5"/>
-        <v>17.741414141414143</v>
+        <v>10.670707070707071</v>
       </c>
       <c r="C37">
         <f t="shared" si="6"/>
-        <v>0.16464646464646465</v>
+        <v>0.3292929292929293</v>
       </c>
       <c r="D37">
         <f t="shared" si="6"/>
-        <v>1.398989898989899</v>
+        <v>2.0808080808080809</v>
       </c>
       <c r="E37">
         <f t="shared" si="7"/>
-        <v>10.303030303030303</v>
+        <v>8.5353535353535364</v>
       </c>
       <c r="F37">
         <f t="shared" si="8"/>
-        <v>13.535353535353536</v>
+        <v>11.767676767676768</v>
       </c>
       <c r="G37">
         <f t="shared" si="9"/>
@@ -3376,7 +3376,7 @@
       </c>
       <c r="M37">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>27.161616161616163</v>
       </c>
       <c r="N37">
         <v>-1</v>
@@ -3398,23 +3398,23 @@
       </c>
       <c r="B38">
         <f t="shared" si="5"/>
-        <v>18.245454545454546</v>
+        <v>10.972727272727273</v>
       </c>
       <c r="C38">
         <f t="shared" si="6"/>
-        <v>0.16363636363636364</v>
+        <v>0.32727272727272727</v>
       </c>
       <c r="D38">
         <f t="shared" si="6"/>
-        <v>1.3818181818181818</v>
+        <v>2.0545454545454547</v>
       </c>
       <c r="E38">
         <f t="shared" si="7"/>
-        <v>10.454545454545455</v>
+        <v>8.6363636363636367</v>
       </c>
       <c r="F38">
         <f t="shared" si="8"/>
-        <v>13.636363636363637</v>
+        <v>11.818181818181818</v>
       </c>
       <c r="G38">
         <f t="shared" si="9"/>
@@ -3439,7 +3439,7 @@
       </c>
       <c r="M38">
         <f t="shared" si="2"/>
-        <v>37</v>
+        <v>27.90909090909091</v>
       </c>
       <c r="N38">
         <v>-1</v>
@@ -3461,23 +3461,23 @@
       </c>
       <c r="B39">
         <f t="shared" si="5"/>
-        <v>18.749494949494952</v>
+        <v>11.274747474747475</v>
       </c>
       <c r="C39">
         <f t="shared" si="6"/>
-        <v>0.16262626262626262</v>
+        <v>0.32525252525252524</v>
       </c>
       <c r="D39">
         <f t="shared" si="6"/>
-        <v>1.3646464646464647</v>
+        <v>2.028282828282828</v>
       </c>
       <c r="E39">
         <f t="shared" si="7"/>
-        <v>10.606060606060606</v>
+        <v>8.737373737373737</v>
       </c>
       <c r="F39">
         <f t="shared" si="8"/>
-        <v>13.737373737373737</v>
+        <v>11.868686868686869</v>
       </c>
       <c r="G39">
         <f t="shared" si="9"/>
@@ -3502,7 +3502,7 @@
       </c>
       <c r="M39">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>28.656565656565657</v>
       </c>
       <c r="N39">
         <v>-1</v>
@@ -3524,23 +3524,23 @@
       </c>
       <c r="B40">
         <f t="shared" si="5"/>
-        <v>19.253535353535352</v>
+        <v>11.576767676767675</v>
       </c>
       <c r="C40">
         <f t="shared" si="6"/>
-        <v>0.16161616161616163</v>
+        <v>0.32323232323232326</v>
       </c>
       <c r="D40">
         <f t="shared" si="6"/>
-        <v>1.3474747474747475</v>
+        <v>2.0020202020202023</v>
       </c>
       <c r="E40">
         <f t="shared" si="7"/>
-        <v>10.757575757575758</v>
+        <v>8.8383838383838373</v>
       </c>
       <c r="F40">
         <f t="shared" si="8"/>
-        <v>13.838383838383837</v>
+        <v>11.919191919191919</v>
       </c>
       <c r="G40">
         <f t="shared" si="9"/>
@@ -3565,7 +3565,7 @@
       </c>
       <c r="M40">
         <f t="shared" si="2"/>
-        <v>39</v>
+        <v>29.404040404040401</v>
       </c>
       <c r="N40">
         <v>-1</v>
@@ -3587,23 +3587,23 @@
       </c>
       <c r="B41">
         <f t="shared" si="5"/>
-        <v>19.757575757575758</v>
+        <v>11.878787878787877</v>
       </c>
       <c r="C41">
         <f t="shared" si="6"/>
-        <v>0.16060606060606061</v>
+        <v>0.32121212121212123</v>
       </c>
       <c r="D41">
         <f t="shared" si="6"/>
-        <v>1.3303030303030303</v>
+        <v>1.9757575757575758</v>
       </c>
       <c r="E41">
         <f t="shared" si="7"/>
-        <v>10.90909090909091</v>
+        <v>8.9393939393939394</v>
       </c>
       <c r="F41">
         <f t="shared" si="8"/>
-        <v>13.939393939393939</v>
+        <v>11.969696969696969</v>
       </c>
       <c r="G41">
         <f t="shared" si="9"/>
@@ -3628,7 +3628,7 @@
       </c>
       <c r="M41">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>30.151515151515149</v>
       </c>
       <c r="N41">
         <v>-1</v>
@@ -3650,23 +3650,23 @@
       </c>
       <c r="B42">
         <f t="shared" si="5"/>
-        <v>20.261616161616161</v>
+        <v>12.180808080808079</v>
       </c>
       <c r="C42">
         <f t="shared" si="6"/>
-        <v>0.1595959595959596</v>
+        <v>0.31919191919191919</v>
       </c>
       <c r="D42">
         <f t="shared" si="6"/>
-        <v>1.3131313131313131</v>
+        <v>1.9494949494949494</v>
       </c>
       <c r="E42">
         <f t="shared" si="7"/>
-        <v>11.060606060606061</v>
+        <v>9.0404040404040416</v>
       </c>
       <c r="F42">
         <f t="shared" si="8"/>
-        <v>14.040404040404042</v>
+        <v>12.020202020202021</v>
       </c>
       <c r="G42">
         <f t="shared" si="9"/>
@@ -3691,7 +3691,7 @@
       </c>
       <c r="M42">
         <f t="shared" si="2"/>
-        <v>41</v>
+        <v>30.8989898989899</v>
       </c>
       <c r="N42">
         <v>-1</v>
@@ -3713,23 +3713,23 @@
       </c>
       <c r="B43">
         <f t="shared" si="5"/>
-        <v>20.765656565656567</v>
+        <v>12.482828282828281</v>
       </c>
       <c r="C43">
         <f t="shared" si="6"/>
-        <v>0.15858585858585861</v>
+        <v>0.31717171717171722</v>
       </c>
       <c r="D43">
         <f t="shared" si="6"/>
-        <v>1.295959595959596</v>
+        <v>1.9232323232323232</v>
       </c>
       <c r="E43">
         <f t="shared" si="7"/>
-        <v>11.212121212121211</v>
+        <v>9.1414141414141419</v>
       </c>
       <c r="F43">
         <f t="shared" si="8"/>
-        <v>14.141414141414142</v>
+        <v>12.070707070707071</v>
       </c>
       <c r="G43">
         <f t="shared" si="9"/>
@@ -3754,7 +3754,7 @@
       </c>
       <c r="M43">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>31.646464646464647</v>
       </c>
       <c r="N43">
         <v>-1</v>
@@ -3776,23 +3776,23 @@
       </c>
       <c r="B44">
         <f t="shared" si="5"/>
-        <v>21.26969696969697</v>
+        <v>12.784848484848485</v>
       </c>
       <c r="C44">
         <f t="shared" si="6"/>
-        <v>0.15757575757575759</v>
+        <v>0.31515151515151518</v>
       </c>
       <c r="D44">
         <f t="shared" si="6"/>
-        <v>1.2787878787878788</v>
+        <v>1.896969696969697</v>
       </c>
       <c r="E44">
         <f t="shared" si="7"/>
-        <v>11.363636363636363</v>
+        <v>9.2424242424242422</v>
       </c>
       <c r="F44">
         <f t="shared" si="8"/>
-        <v>14.242424242424242</v>
+        <v>12.121212121212121</v>
       </c>
       <c r="G44">
         <f t="shared" si="9"/>
@@ -3817,7 +3817,7 @@
       </c>
       <c r="M44">
         <f t="shared" si="2"/>
-        <v>43</v>
+        <v>32.393939393939391</v>
       </c>
       <c r="N44">
         <v>-1</v>
@@ -3839,23 +3839,23 @@
       </c>
       <c r="B45">
         <f t="shared" si="5"/>
-        <v>21.773737373737376</v>
+        <v>13.086868686868687</v>
       </c>
       <c r="C45">
         <f t="shared" si="6"/>
-        <v>0.15656565656565657</v>
+        <v>0.31313131313131315</v>
       </c>
       <c r="D45">
         <f t="shared" si="6"/>
-        <v>1.2616161616161616</v>
+        <v>1.8707070707070705</v>
       </c>
       <c r="E45">
         <f t="shared" si="7"/>
-        <v>11.515151515151516</v>
+        <v>9.3434343434343425</v>
       </c>
       <c r="F45">
         <f t="shared" si="8"/>
-        <v>14.343434343434343</v>
+        <v>12.171717171717171</v>
       </c>
       <c r="G45">
         <f t="shared" si="9"/>
@@ -3880,7 +3880,7 @@
       </c>
       <c r="M45">
         <f t="shared" si="2"/>
-        <v>44</v>
+        <v>33.141414141414145</v>
       </c>
       <c r="N45">
         <v>-1</v>
@@ -3902,23 +3902,23 @@
       </c>
       <c r="B46">
         <f t="shared" si="5"/>
-        <v>22.277777777777779</v>
+        <v>13.388888888888888</v>
       </c>
       <c r="C46">
         <f t="shared" ref="C46:C77" si="11">(C$2+((SUM(A46-1)/SUM(A$101-1))*(SUM(C$101-C$2))))</f>
-        <v>0.15555555555555556</v>
+        <v>0.31111111111111112</v>
       </c>
       <c r="D46">
         <f t="shared" si="6"/>
-        <v>1.2444444444444445</v>
+        <v>1.8444444444444446</v>
       </c>
       <c r="E46">
         <f t="shared" si="7"/>
-        <v>11.666666666666666</v>
+        <v>9.4444444444444446</v>
       </c>
       <c r="F46">
         <f t="shared" si="8"/>
-        <v>14.444444444444445</v>
+        <v>12.222222222222221</v>
       </c>
       <c r="G46">
         <f t="shared" si="9"/>
@@ -3943,7 +3943,7 @@
       </c>
       <c r="M46">
         <f t="shared" si="2"/>
-        <v>45</v>
+        <v>33.888888888888886</v>
       </c>
       <c r="N46">
         <v>-1</v>
@@ -3965,23 +3965,23 @@
       </c>
       <c r="B47">
         <f t="shared" si="5"/>
-        <v>22.781818181818181</v>
+        <v>13.69090909090909</v>
       </c>
       <c r="C47">
         <f t="shared" si="11"/>
-        <v>0.15454545454545454</v>
+        <v>0.30909090909090908</v>
       </c>
       <c r="D47">
         <f t="shared" ref="D47:D100" si="12">(D$2+((SUM($A47-1)/SUM($A$101-1))*(SUM(D$101-D$2))))</f>
-        <v>1.2272727272727273</v>
+        <v>1.8181818181818181</v>
       </c>
       <c r="E47">
         <f t="shared" si="7"/>
-        <v>11.818181818181818</v>
+        <v>9.545454545454545</v>
       </c>
       <c r="F47">
         <f t="shared" si="8"/>
-        <v>14.545454545454545</v>
+        <v>12.272727272727273</v>
       </c>
       <c r="G47">
         <f t="shared" si="9"/>
@@ -4006,7 +4006,7 @@
       </c>
       <c r="M47">
         <f t="shared" si="2"/>
-        <v>46</v>
+        <v>34.636363636363633</v>
       </c>
       <c r="N47">
         <v>-1</v>
@@ -4028,23 +4028,23 @@
       </c>
       <c r="B48">
         <f t="shared" si="5"/>
-        <v>23.285858585858588</v>
+        <v>13.992929292929292</v>
       </c>
       <c r="C48">
         <f t="shared" si="11"/>
-        <v>0.15353535353535355</v>
+        <v>0.30707070707070711</v>
       </c>
       <c r="D48">
         <f t="shared" si="12"/>
-        <v>1.2101010101010101</v>
+        <v>1.7919191919191919</v>
       </c>
       <c r="E48">
         <f t="shared" si="7"/>
-        <v>11.969696969696969</v>
+        <v>9.6464646464646471</v>
       </c>
       <c r="F48">
         <f t="shared" si="8"/>
-        <v>14.646464646464647</v>
+        <v>12.323232323232324</v>
       </c>
       <c r="G48">
         <f t="shared" si="9"/>
@@ -4069,7 +4069,7 @@
       </c>
       <c r="M48">
         <f t="shared" si="2"/>
-        <v>47</v>
+        <v>35.383838383838381</v>
       </c>
       <c r="N48">
         <v>-1</v>
@@ -4091,23 +4091,23 @@
       </c>
       <c r="B49">
         <f t="shared" si="5"/>
-        <v>23.78989898989899</v>
+        <v>14.294949494949494</v>
       </c>
       <c r="C49">
         <f t="shared" si="11"/>
-        <v>0.15252525252525254</v>
+        <v>0.30505050505050507</v>
       </c>
       <c r="D49">
         <f t="shared" si="12"/>
-        <v>1.192929292929293</v>
+        <v>1.7656565656565657</v>
       </c>
       <c r="E49">
         <f t="shared" si="7"/>
-        <v>12.121212121212121</v>
+        <v>9.7474747474747474</v>
       </c>
       <c r="F49">
         <f t="shared" si="8"/>
-        <v>14.747474747474747</v>
+        <v>12.373737373737374</v>
       </c>
       <c r="G49">
         <f t="shared" si="9"/>
@@ -4132,7 +4132,7 @@
       </c>
       <c r="M49">
         <f t="shared" si="2"/>
-        <v>48</v>
+        <v>36.131313131313135</v>
       </c>
       <c r="N49">
         <v>-1</v>
@@ -4154,23 +4154,23 @@
       </c>
       <c r="B50">
         <f t="shared" si="5"/>
-        <v>24.293939393939397</v>
+        <v>14.596969696969696</v>
       </c>
       <c r="C50">
         <f t="shared" si="11"/>
-        <v>0.15151515151515152</v>
+        <v>0.30303030303030304</v>
       </c>
       <c r="D50">
         <f t="shared" si="12"/>
-        <v>1.1757575757575758</v>
+        <v>1.7393939393939393</v>
       </c>
       <c r="E50">
         <f t="shared" si="7"/>
-        <v>12.272727272727273</v>
+        <v>9.8484848484848477</v>
       </c>
       <c r="F50">
         <f t="shared" si="8"/>
-        <v>14.848484848484848</v>
+        <v>12.424242424242424</v>
       </c>
       <c r="G50">
         <f t="shared" si="9"/>
@@ -4195,7 +4195,7 @@
       </c>
       <c r="M50">
         <f t="shared" si="2"/>
-        <v>49</v>
+        <v>36.878787878787882</v>
       </c>
       <c r="N50">
         <v>-1</v>
@@ -4217,23 +4217,23 @@
       </c>
       <c r="B51">
         <f t="shared" si="5"/>
-        <v>24.797979797979799</v>
+        <v>14.898989898989898</v>
       </c>
       <c r="C51">
         <f t="shared" si="11"/>
-        <v>0.1505050505050505</v>
+        <v>0.30101010101010101</v>
       </c>
       <c r="D51">
         <f t="shared" si="12"/>
-        <v>1.1585858585858586</v>
+        <v>1.7131313131313131</v>
       </c>
       <c r="E51">
         <f t="shared" si="7"/>
-        <v>12.424242424242426</v>
+        <v>9.9494949494949498</v>
       </c>
       <c r="F51">
         <f t="shared" si="8"/>
-        <v>14.94949494949495</v>
+        <v>12.474747474747474</v>
       </c>
       <c r="G51">
         <f t="shared" si="9"/>
@@ -4258,7 +4258,7 @@
       </c>
       <c r="M51">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>37.62626262626263</v>
       </c>
       <c r="N51">
         <v>-1</v>
@@ -4280,23 +4280,23 @@
       </c>
       <c r="B52">
         <f t="shared" si="5"/>
-        <v>25.302020202020206</v>
+        <v>15.201010101010102</v>
       </c>
       <c r="C52">
         <f t="shared" si="11"/>
-        <v>0.14949494949494951</v>
+        <v>0.29898989898989903</v>
       </c>
       <c r="D52">
         <f t="shared" si="12"/>
-        <v>1.1414141414141414</v>
+        <v>1.6868686868686866</v>
       </c>
       <c r="E52">
         <f t="shared" si="7"/>
-        <v>12.575757575757576</v>
+        <v>10.050505050505052</v>
       </c>
       <c r="F52">
         <f t="shared" si="8"/>
-        <v>15.050505050505052</v>
+        <v>12.525252525252526</v>
       </c>
       <c r="G52">
         <f t="shared" si="9"/>
@@ -4321,7 +4321,7 @@
       </c>
       <c r="M52">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>38.373737373737377</v>
       </c>
       <c r="N52">
         <v>-1</v>
@@ -4343,23 +4343,23 @@
       </c>
       <c r="B53">
         <f t="shared" si="5"/>
-        <v>25.806060606060605</v>
+        <v>15.503030303030302</v>
       </c>
       <c r="C53">
         <f t="shared" si="11"/>
-        <v>0.1484848484848485</v>
+        <v>0.29696969696969699</v>
       </c>
       <c r="D53">
         <f t="shared" si="12"/>
-        <v>1.1242424242424243</v>
+        <v>1.6606060606060606</v>
       </c>
       <c r="E53">
         <f t="shared" si="7"/>
-        <v>12.727272727272727</v>
+        <v>10.151515151515152</v>
       </c>
       <c r="F53">
         <f t="shared" si="8"/>
-        <v>15.151515151515152</v>
+        <v>12.575757575757576</v>
       </c>
       <c r="G53">
         <f t="shared" si="9"/>
@@ -4384,7 +4384,7 @@
       </c>
       <c r="M53">
         <f t="shared" si="2"/>
-        <v>52</v>
+        <v>39.121212121212118</v>
       </c>
       <c r="N53">
         <v>-1</v>
@@ -4406,23 +4406,23 @@
       </c>
       <c r="B54">
         <f t="shared" si="5"/>
-        <v>26.310101010101015</v>
+        <v>15.805050505050506</v>
       </c>
       <c r="C54">
         <f t="shared" si="11"/>
-        <v>0.14747474747474748</v>
+        <v>0.29494949494949496</v>
       </c>
       <c r="D54">
         <f t="shared" si="12"/>
-        <v>1.1070707070707071</v>
+        <v>1.6343434343434342</v>
       </c>
       <c r="E54">
         <f t="shared" si="7"/>
-        <v>12.878787878787879</v>
+        <v>10.252525252525253</v>
       </c>
       <c r="F54">
         <f t="shared" si="8"/>
-        <v>15.252525252525253</v>
+        <v>12.626262626262626</v>
       </c>
       <c r="G54">
         <f t="shared" si="9"/>
@@ -4447,7 +4447,7 @@
       </c>
       <c r="M54">
         <f t="shared" si="2"/>
-        <v>53.000000000000007</v>
+        <v>39.868686868686872</v>
       </c>
       <c r="N54">
         <v>-1</v>
@@ -4469,23 +4469,23 @@
       </c>
       <c r="B55">
         <f t="shared" si="5"/>
-        <v>26.814141414141414</v>
+        <v>16.107070707070708</v>
       </c>
       <c r="C55">
         <f t="shared" si="11"/>
-        <v>0.14646464646464646</v>
+        <v>0.29292929292929293</v>
       </c>
       <c r="D55">
         <f t="shared" si="12"/>
-        <v>1.0898989898989899</v>
+        <v>1.608080808080808</v>
       </c>
       <c r="E55">
         <f t="shared" si="7"/>
-        <v>13.030303030303031</v>
+        <v>10.353535353535353</v>
       </c>
       <c r="F55">
         <f t="shared" si="8"/>
-        <v>15.353535353535353</v>
+        <v>12.676767676767676</v>
       </c>
       <c r="G55">
         <f t="shared" si="9"/>
@@ -4510,7 +4510,7 @@
       </c>
       <c r="M55">
         <f t="shared" si="2"/>
-        <v>54</v>
+        <v>40.616161616161619</v>
       </c>
       <c r="N55">
         <v>-1</v>
@@ -4532,23 +4532,23 @@
       </c>
       <c r="B56">
         <f t="shared" si="5"/>
-        <v>27.318181818181817</v>
+        <v>16.40909090909091</v>
       </c>
       <c r="C56">
         <f t="shared" si="11"/>
-        <v>0.14545454545454548</v>
+        <v>0.29090909090909095</v>
       </c>
       <c r="D56">
         <f t="shared" si="12"/>
-        <v>1.0727272727272728</v>
+        <v>1.5818181818181818</v>
       </c>
       <c r="E56">
         <f t="shared" si="7"/>
-        <v>13.181818181818182</v>
+        <v>10.454545454545453</v>
       </c>
       <c r="F56">
         <f t="shared" si="8"/>
-        <v>15.454545454545453</v>
+        <v>12.727272727272727</v>
       </c>
       <c r="G56">
         <f t="shared" si="9"/>
@@ -4573,7 +4573,7 @@
       </c>
       <c r="M56">
         <f t="shared" si="2"/>
-        <v>54.999999999999993</v>
+        <v>41.36363636363636</v>
       </c>
       <c r="N56">
         <v>-1</v>
@@ -4595,23 +4595,23 @@
       </c>
       <c r="B57">
         <f t="shared" si="5"/>
-        <v>27.822222222222223</v>
+        <v>16.711111111111112</v>
       </c>
       <c r="C57">
         <f t="shared" si="11"/>
-        <v>0.14444444444444446</v>
+        <v>0.28888888888888892</v>
       </c>
       <c r="D57">
         <f t="shared" si="12"/>
-        <v>1.0555555555555556</v>
+        <v>1.5555555555555554</v>
       </c>
       <c r="E57">
         <f t="shared" si="7"/>
-        <v>13.333333333333334</v>
+        <v>10.555555555555555</v>
       </c>
       <c r="F57">
         <f t="shared" si="8"/>
-        <v>15.555555555555555</v>
+        <v>12.777777777777779</v>
       </c>
       <c r="G57">
         <f t="shared" si="9"/>
@@ -4636,7 +4636,7 @@
       </c>
       <c r="M57">
         <f t="shared" si="2"/>
-        <v>56</v>
+        <v>42.111111111111114</v>
       </c>
       <c r="N57">
         <v>-1</v>
@@ -4658,23 +4658,23 @@
       </c>
       <c r="B58">
         <f t="shared" si="5"/>
-        <v>28.326262626262626</v>
+        <v>17.013131313131314</v>
       </c>
       <c r="C58">
         <f t="shared" si="11"/>
-        <v>0.14343434343434344</v>
+        <v>0.28686868686868688</v>
       </c>
       <c r="D58">
         <f t="shared" si="12"/>
-        <v>1.0383838383838384</v>
+        <v>1.5292929292929294</v>
       </c>
       <c r="E58">
         <f t="shared" si="7"/>
-        <v>13.484848484848484</v>
+        <v>10.656565656565657</v>
       </c>
       <c r="F58">
         <f t="shared" si="8"/>
-        <v>15.656565656565657</v>
+        <v>12.828282828282829</v>
       </c>
       <c r="G58">
         <f t="shared" si="9"/>
@@ -4699,7 +4699,7 @@
       </c>
       <c r="M58">
         <f t="shared" si="2"/>
-        <v>57</v>
+        <v>42.858585858585855</v>
       </c>
       <c r="N58">
         <v>-1</v>
@@ -4721,23 +4721,23 @@
       </c>
       <c r="B59">
         <f t="shared" si="5"/>
-        <v>28.830303030303032</v>
+        <v>17.315151515151516</v>
       </c>
       <c r="C59">
         <f t="shared" si="11"/>
-        <v>0.14242424242424243</v>
+        <v>0.28484848484848485</v>
       </c>
       <c r="D59">
         <f t="shared" si="12"/>
-        <v>1.021212121212121</v>
+        <v>1.5030303030303029</v>
       </c>
       <c r="E59">
         <f t="shared" si="7"/>
-        <v>13.636363636363637</v>
+        <v>10.757575757575758</v>
       </c>
       <c r="F59">
         <f t="shared" si="8"/>
-        <v>15.757575757575758</v>
+        <v>12.878787878787879</v>
       </c>
       <c r="G59">
         <f t="shared" si="9"/>
@@ -4762,7 +4762,7 @@
       </c>
       <c r="M59">
         <f t="shared" si="2"/>
-        <v>58.000000000000007</v>
+        <v>43.606060606060609</v>
       </c>
       <c r="N59">
         <v>-1</v>
@@ -4784,23 +4784,23 @@
       </c>
       <c r="B60">
         <f t="shared" si="5"/>
-        <v>29.334343434343435</v>
+        <v>17.617171717171718</v>
       </c>
       <c r="C60">
         <f t="shared" si="11"/>
-        <v>0.14141414141414144</v>
+        <v>0.28282828282828287</v>
       </c>
       <c r="D60">
         <f t="shared" si="12"/>
-        <v>1.0040404040404041</v>
+        <v>1.4767676767676767</v>
       </c>
       <c r="E60">
         <f t="shared" si="7"/>
-        <v>13.787878787878787</v>
+        <v>10.858585858585858</v>
       </c>
       <c r="F60">
         <f t="shared" si="8"/>
-        <v>15.858585858585858</v>
+        <v>12.929292929292929</v>
       </c>
       <c r="G60">
         <f t="shared" si="9"/>
@@ -4825,7 +4825,7 @@
       </c>
       <c r="M60">
         <f t="shared" si="2"/>
-        <v>59</v>
+        <v>44.353535353535356</v>
       </c>
       <c r="N60">
         <v>-1</v>
@@ -4847,23 +4847,23 @@
       </c>
       <c r="B61">
         <f t="shared" si="5"/>
-        <v>29.838383838383837</v>
+        <v>17.919191919191917</v>
       </c>
       <c r="C61">
         <f t="shared" si="11"/>
-        <v>0.14040404040404042</v>
+        <v>0.28080808080808084</v>
       </c>
       <c r="D61">
         <f t="shared" si="12"/>
-        <v>0.9868686868686869</v>
+        <v>1.4505050505050505</v>
       </c>
       <c r="E61">
         <f t="shared" si="7"/>
-        <v>13.939393939393939</v>
+        <v>10.959595959595958</v>
       </c>
       <c r="F61">
         <f t="shared" si="8"/>
-        <v>15.959595959595958</v>
+        <v>12.979797979797979</v>
       </c>
       <c r="G61">
         <f t="shared" si="9"/>
@@ -4888,7 +4888,7 @@
       </c>
       <c r="M61">
         <f t="shared" si="2"/>
-        <v>59.999999999999993</v>
+        <v>45.101010101010097</v>
       </c>
       <c r="N61">
         <v>-1</v>
@@ -4910,23 +4910,23 @@
       </c>
       <c r="B62">
         <f t="shared" si="5"/>
-        <v>30.342424242424244</v>
+        <v>18.221212121212123</v>
       </c>
       <c r="C62">
         <f t="shared" si="11"/>
-        <v>0.1393939393939394</v>
+        <v>0.27878787878787881</v>
       </c>
       <c r="D62">
         <f t="shared" si="12"/>
-        <v>0.96969696969696972</v>
+        <v>1.4242424242424241</v>
       </c>
       <c r="E62">
         <f t="shared" si="7"/>
-        <v>14.090909090909092</v>
+        <v>11.060606060606061</v>
       </c>
       <c r="F62">
         <f t="shared" si="8"/>
-        <v>16.060606060606062</v>
+        <v>13.030303030303031</v>
       </c>
       <c r="G62">
         <f t="shared" si="9"/>
@@ -4951,7 +4951,7 @@
       </c>
       <c r="M62">
         <f t="shared" si="2"/>
-        <v>61</v>
+        <v>45.848484848484851</v>
       </c>
       <c r="N62">
         <v>-1</v>
@@ -4973,23 +4973,23 @@
       </c>
       <c r="B63">
         <f t="shared" si="5"/>
-        <v>30.846464646464646</v>
+        <v>18.523232323232325</v>
       </c>
       <c r="C63">
         <f t="shared" si="11"/>
-        <v>0.13838383838383839</v>
+        <v>0.27676767676767677</v>
       </c>
       <c r="D63">
         <f t="shared" si="12"/>
-        <v>0.95252525252525255</v>
+        <v>1.3979797979797981</v>
       </c>
       <c r="E63">
         <f t="shared" si="7"/>
-        <v>14.242424242424242</v>
+        <v>11.161616161616161</v>
       </c>
       <c r="F63">
         <f t="shared" si="8"/>
-        <v>16.161616161616159</v>
+        <v>13.08080808080808</v>
       </c>
       <c r="G63">
         <f t="shared" si="9"/>
@@ -5014,7 +5014,7 @@
       </c>
       <c r="M63">
         <f t="shared" si="2"/>
-        <v>62</v>
+        <v>46.595959595959592</v>
       </c>
       <c r="N63">
         <v>-1</v>
@@ -5036,23 +5036,23 @@
       </c>
       <c r="B64">
         <f t="shared" si="5"/>
-        <v>31.350505050505053</v>
+        <v>18.825252525252527</v>
       </c>
       <c r="C64">
         <f t="shared" si="11"/>
-        <v>0.13737373737373737</v>
+        <v>0.27474747474747474</v>
       </c>
       <c r="D64">
         <f t="shared" si="12"/>
-        <v>0.93535353535353538</v>
+        <v>1.3717171717171717</v>
       </c>
       <c r="E64">
         <f t="shared" si="7"/>
-        <v>14.393939393939394</v>
+        <v>11.262626262626263</v>
       </c>
       <c r="F64">
         <f t="shared" si="8"/>
-        <v>16.262626262626263</v>
+        <v>13.131313131313131</v>
       </c>
       <c r="G64">
         <f t="shared" si="9"/>
@@ -5077,7 +5077,7 @@
       </c>
       <c r="M64">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>47.343434343434346</v>
       </c>
       <c r="N64">
         <v>-1</v>
@@ -5099,23 +5099,23 @@
       </c>
       <c r="B65">
         <f t="shared" si="5"/>
-        <v>31.854545454545455</v>
+        <v>19.127272727272729</v>
       </c>
       <c r="C65">
         <f t="shared" si="11"/>
-        <v>0.13636363636363635</v>
+        <v>0.27272727272727271</v>
       </c>
       <c r="D65">
         <f t="shared" si="12"/>
-        <v>0.91818181818181821</v>
+        <v>1.3454545454545455</v>
       </c>
       <c r="E65">
         <f t="shared" si="7"/>
-        <v>14.545454545454545</v>
+        <v>11.363636363636363</v>
       </c>
       <c r="F65">
         <f t="shared" si="8"/>
-        <v>16.363636363636363</v>
+        <v>13.181818181818182</v>
       </c>
       <c r="G65">
         <f t="shared" si="9"/>
@@ -5140,7 +5140,7 @@
       </c>
       <c r="M65">
         <f t="shared" si="2"/>
-        <v>64</v>
+        <v>48.090909090909093</v>
       </c>
       <c r="N65">
         <v>-1</v>
@@ -5162,23 +5162,23 @@
       </c>
       <c r="B66">
         <f t="shared" si="5"/>
-        <v>32.358585858585862</v>
+        <v>19.429292929292931</v>
       </c>
       <c r="C66">
         <f t="shared" si="11"/>
-        <v>0.13535353535353534</v>
+        <v>0.27070707070707067</v>
       </c>
       <c r="D66">
         <f t="shared" si="12"/>
-        <v>0.90101010101010104</v>
+        <v>1.319191919191919</v>
       </c>
       <c r="E66">
         <f t="shared" si="7"/>
-        <v>14.696969696969697</v>
+        <v>11.464646464646465</v>
       </c>
       <c r="F66">
         <f t="shared" si="8"/>
-        <v>16.464646464646464</v>
+        <v>13.232323232323232</v>
       </c>
       <c r="G66">
         <f t="shared" si="9"/>
@@ -5203,7 +5203,7 @@
       </c>
       <c r="M66">
         <f t="shared" si="2"/>
-        <v>65</v>
+        <v>48.838383838383841</v>
       </c>
       <c r="N66">
         <v>-1</v>
@@ -5225,23 +5225,23 @@
       </c>
       <c r="B67">
         <f t="shared" si="5"/>
-        <v>32.862626262626264</v>
+        <v>19.731313131313133</v>
       </c>
       <c r="C67">
         <f t="shared" si="11"/>
-        <v>0.13434343434343435</v>
+        <v>0.2686868686868687</v>
       </c>
       <c r="D67">
         <f t="shared" si="12"/>
-        <v>0.88383838383838387</v>
+        <v>1.2929292929292928</v>
       </c>
       <c r="E67">
         <f t="shared" si="7"/>
-        <v>14.848484848484848</v>
+        <v>11.565656565656566</v>
       </c>
       <c r="F67">
         <f t="shared" si="8"/>
-        <v>16.565656565656568</v>
+        <v>13.282828282828284</v>
       </c>
       <c r="G67">
         <f t="shared" si="9"/>
@@ -5266,7 +5266,7 @@
       </c>
       <c r="M67">
         <f t="shared" ref="M67:O100" si="13">(M$2+((SUM($A67-1)/SUM($A$101-1))*(SUM(M$101-M$2))))</f>
-        <v>66</v>
+        <v>49.585858585858588</v>
       </c>
       <c r="N67">
         <v>-1</v>
@@ -5288,23 +5288,23 @@
       </c>
       <c r="B68">
         <f t="shared" ref="B68:B100" si="14">(B$2+((SUM(A68-1)/SUM(A$101-1))*(SUM(B$101-B$2))))</f>
-        <v>33.366666666666667</v>
+        <v>20.033333333333331</v>
       </c>
       <c r="C68">
         <f t="shared" si="11"/>
-        <v>0.13333333333333336</v>
+        <v>0.26666666666666672</v>
       </c>
       <c r="D68">
         <f t="shared" si="12"/>
-        <v>0.8666666666666667</v>
+        <v>1.2666666666666666</v>
       </c>
       <c r="E68">
         <f t="shared" si="7"/>
-        <v>15</v>
+        <v>11.666666666666666</v>
       </c>
       <c r="F68">
         <f t="shared" si="8"/>
-        <v>16.666666666666664</v>
+        <v>13.333333333333332</v>
       </c>
       <c r="G68">
         <f t="shared" si="9"/>
@@ -5329,7 +5329,7 @@
       </c>
       <c r="M68">
         <f t="shared" si="13"/>
-        <v>67</v>
+        <v>50.333333333333329</v>
       </c>
       <c r="N68">
         <v>-1</v>
@@ -5351,23 +5351,23 @@
       </c>
       <c r="B69">
         <f t="shared" si="14"/>
-        <v>33.87070707070707</v>
+        <v>20.335353535353537</v>
       </c>
       <c r="C69">
         <f t="shared" si="11"/>
-        <v>0.13232323232323234</v>
+        <v>0.26464646464646469</v>
       </c>
       <c r="D69">
         <f t="shared" si="12"/>
-        <v>0.84949494949494953</v>
+        <v>1.2404040404040402</v>
       </c>
       <c r="E69">
         <f t="shared" si="7"/>
-        <v>15.151515151515152</v>
+        <v>11.767676767676768</v>
       </c>
       <c r="F69">
         <f t="shared" si="8"/>
-        <v>16.767676767676768</v>
+        <v>13.383838383838384</v>
       </c>
       <c r="G69">
         <f t="shared" si="9"/>
@@ -5392,7 +5392,7 @@
       </c>
       <c r="M69">
         <f t="shared" si="13"/>
-        <v>68</v>
+        <v>51.080808080808083</v>
       </c>
       <c r="N69">
         <v>-1</v>
@@ -5414,23 +5414,23 @@
       </c>
       <c r="B70">
         <f t="shared" si="14"/>
-        <v>34.374747474747473</v>
+        <v>20.637373737373736</v>
       </c>
       <c r="C70">
         <f t="shared" si="11"/>
-        <v>0.13131313131313133</v>
+        <v>0.26262626262626265</v>
       </c>
       <c r="D70">
         <f t="shared" si="12"/>
-        <v>0.83232323232323235</v>
+        <v>1.2141414141414142</v>
       </c>
       <c r="E70">
         <f t="shared" si="7"/>
-        <v>15.303030303030303</v>
+        <v>11.868686868686869</v>
       </c>
       <c r="F70">
         <f t="shared" si="8"/>
-        <v>16.868686868686869</v>
+        <v>13.434343434343434</v>
       </c>
       <c r="G70">
         <f t="shared" si="9"/>
@@ -5455,7 +5455,7 @@
       </c>
       <c r="M70">
         <f t="shared" si="13"/>
-        <v>69</v>
+        <v>51.828282828282823</v>
       </c>
       <c r="N70">
         <v>-1</v>
@@ -5477,23 +5477,23 @@
       </c>
       <c r="B71">
         <f t="shared" si="14"/>
-        <v>34.878787878787882</v>
+        <v>20.939393939393941</v>
       </c>
       <c r="C71">
         <f t="shared" si="11"/>
-        <v>0.13030303030303031</v>
+        <v>0.26060606060606062</v>
       </c>
       <c r="D71">
         <f t="shared" si="12"/>
-        <v>0.81515151515151518</v>
+        <v>1.1878787878787878</v>
       </c>
       <c r="E71">
         <f t="shared" si="7"/>
-        <v>15.454545454545455</v>
+        <v>11.969696969696971</v>
       </c>
       <c r="F71">
         <f t="shared" si="8"/>
-        <v>16.969696969696969</v>
+        <v>13.484848484848484</v>
       </c>
       <c r="G71">
         <f t="shared" si="9"/>
@@ -5518,7 +5518,7 @@
       </c>
       <c r="M71">
         <f t="shared" si="13"/>
-        <v>70</v>
+        <v>52.575757575757578</v>
       </c>
       <c r="N71">
         <v>-1</v>
@@ -5540,23 +5540,23 @@
       </c>
       <c r="B72">
         <f t="shared" si="14"/>
-        <v>35.382828282828285</v>
+        <v>21.241414141414143</v>
       </c>
       <c r="C72">
         <f t="shared" si="11"/>
-        <v>0.12929292929292929</v>
+        <v>0.25858585858585859</v>
       </c>
       <c r="D72">
         <f t="shared" si="12"/>
-        <v>0.79797979797979801</v>
+        <v>1.1616161616161615</v>
       </c>
       <c r="E72">
         <f t="shared" si="7"/>
-        <v>15.606060606060606</v>
+        <v>12.070707070707071</v>
       </c>
       <c r="F72">
         <f t="shared" si="8"/>
-        <v>17.070707070707073</v>
+        <v>13.535353535353536</v>
       </c>
       <c r="G72">
         <f t="shared" si="9"/>
@@ -5581,7 +5581,7 @@
       </c>
       <c r="M72">
         <f t="shared" si="13"/>
-        <v>71</v>
+        <v>53.323232323232325</v>
       </c>
       <c r="N72">
         <v>-1</v>
@@ -5603,23 +5603,23 @@
       </c>
       <c r="B73">
         <f t="shared" si="14"/>
-        <v>35.886868686868688</v>
+        <v>21.543434343434342</v>
       </c>
       <c r="C73">
         <f t="shared" si="11"/>
-        <v>0.12828282828282828</v>
+        <v>0.25656565656565655</v>
       </c>
       <c r="D73">
         <f t="shared" si="12"/>
-        <v>0.78080808080808084</v>
+        <v>1.1353535353535353</v>
       </c>
       <c r="E73">
         <f t="shared" si="7"/>
-        <v>15.757575757575758</v>
+        <v>12.171717171717171</v>
       </c>
       <c r="F73">
         <f t="shared" si="8"/>
-        <v>17.171717171717169</v>
+        <v>13.585858585858585</v>
       </c>
       <c r="G73">
         <f t="shared" si="9"/>
@@ -5644,7 +5644,7 @@
       </c>
       <c r="M73">
         <f t="shared" si="13"/>
-        <v>72</v>
+        <v>54.070707070707066</v>
       </c>
       <c r="N73">
         <v>-1</v>
@@ -5666,23 +5666,23 @@
       </c>
       <c r="B74">
         <f t="shared" si="14"/>
-        <v>36.390909090909091</v>
+        <v>21.845454545454547</v>
       </c>
       <c r="C74">
         <f t="shared" si="11"/>
-        <v>0.12727272727272726</v>
+        <v>0.25454545454545452</v>
       </c>
       <c r="D74">
         <f t="shared" si="12"/>
-        <v>0.76363636363636367</v>
+        <v>1.1090909090909089</v>
       </c>
       <c r="E74">
         <f t="shared" si="7"/>
-        <v>15.90909090909091</v>
+        <v>12.272727272727273</v>
       </c>
       <c r="F74">
         <f t="shared" si="8"/>
-        <v>17.272727272727273</v>
+        <v>13.636363636363637</v>
       </c>
       <c r="G74">
         <f t="shared" si="9"/>
@@ -5707,7 +5707,7 @@
       </c>
       <c r="M74">
         <f t="shared" si="13"/>
-        <v>73</v>
+        <v>54.81818181818182</v>
       </c>
       <c r="N74">
         <v>-1</v>
@@ -5729,23 +5729,23 @@
       </c>
       <c r="B75">
         <f t="shared" si="14"/>
-        <v>36.894949494949493</v>
+        <v>22.147474747474746</v>
       </c>
       <c r="C75">
         <f t="shared" si="11"/>
-        <v>0.12626262626262627</v>
+        <v>0.25252525252525254</v>
       </c>
       <c r="D75">
         <f t="shared" si="12"/>
-        <v>0.7464646464646465</v>
+        <v>1.0828282828282829</v>
       </c>
       <c r="E75">
         <f t="shared" si="7"/>
-        <v>16.060606060606062</v>
+        <v>12.373737373737374</v>
       </c>
       <c r="F75">
         <f t="shared" si="8"/>
-        <v>17.373737373737374</v>
+        <v>13.686868686868687</v>
       </c>
       <c r="G75">
         <f t="shared" si="9"/>
@@ -5770,7 +5770,7 @@
       </c>
       <c r="M75">
         <f t="shared" si="13"/>
-        <v>74</v>
+        <v>55.56565656565656</v>
       </c>
       <c r="N75">
         <v>-1</v>
@@ -5792,23 +5792,23 @@
       </c>
       <c r="B76">
         <f t="shared" si="14"/>
-        <v>37.398989898989903</v>
+        <v>22.449494949494952</v>
       </c>
       <c r="C76">
         <f t="shared" si="11"/>
-        <v>0.12525252525252525</v>
+        <v>0.25050505050505051</v>
       </c>
       <c r="D76">
         <f t="shared" si="12"/>
-        <v>0.72929292929292933</v>
+        <v>1.0565656565656565</v>
       </c>
       <c r="E76">
         <f t="shared" si="7"/>
-        <v>16.212121212121211</v>
+        <v>12.474747474747474</v>
       </c>
       <c r="F76">
         <f t="shared" si="8"/>
-        <v>17.474747474747474</v>
+        <v>13.737373737373737</v>
       </c>
       <c r="G76">
         <f t="shared" si="9"/>
@@ -5833,7 +5833,7 @@
       </c>
       <c r="M76">
         <f t="shared" si="13"/>
-        <v>75</v>
+        <v>56.313131313131315</v>
       </c>
       <c r="N76">
         <v>-1</v>
@@ -5855,23 +5855,23 @@
       </c>
       <c r="B77">
         <f t="shared" si="14"/>
-        <v>37.903030303030306</v>
+        <v>22.75151515151515</v>
       </c>
       <c r="C77">
         <f t="shared" si="11"/>
-        <v>0.12424242424242425</v>
+        <v>0.2484848484848485</v>
       </c>
       <c r="D77">
         <f t="shared" si="12"/>
-        <v>0.71212121212121215</v>
+        <v>1.0303030303030303</v>
       </c>
       <c r="E77">
         <f t="shared" si="7"/>
-        <v>16.363636363636363</v>
+        <v>12.575757575757576</v>
       </c>
       <c r="F77">
         <f t="shared" si="8"/>
-        <v>17.575757575757578</v>
+        <v>13.787878787878789</v>
       </c>
       <c r="G77">
         <f t="shared" si="9"/>
@@ -5896,7 +5896,7 @@
       </c>
       <c r="M77">
         <f t="shared" si="13"/>
-        <v>76</v>
+        <v>57.060606060606062</v>
       </c>
       <c r="N77">
         <v>-1</v>
@@ -5918,23 +5918,23 @@
       </c>
       <c r="B78">
         <f t="shared" si="14"/>
-        <v>38.407070707070702</v>
+        <v>23.053535353535352</v>
       </c>
       <c r="C78">
         <f t="shared" ref="C78:C100" si="15">(C$2+((SUM(A78-1)/SUM(A$101-1))*(SUM(C$101-C$2))))</f>
-        <v>0.12323232323232325</v>
+        <v>0.2464646464646465</v>
       </c>
       <c r="D78">
         <f t="shared" si="12"/>
-        <v>0.69494949494949498</v>
+        <v>1.0040404040404041</v>
       </c>
       <c r="E78">
         <f t="shared" si="7"/>
-        <v>16.515151515151516</v>
+        <v>12.676767676767676</v>
       </c>
       <c r="F78">
         <f t="shared" si="8"/>
-        <v>17.676767676767675</v>
+        <v>13.838383838383837</v>
       </c>
       <c r="G78">
         <f t="shared" si="9"/>
@@ -5959,7 +5959,7 @@
       </c>
       <c r="M78">
         <f t="shared" si="13"/>
-        <v>77</v>
+        <v>57.808080808080803</v>
       </c>
       <c r="N78">
         <v>-1</v>
@@ -5981,23 +5981,23 @@
       </c>
       <c r="B79">
         <f t="shared" si="14"/>
-        <v>38.911111111111111</v>
+        <v>23.355555555555558</v>
       </c>
       <c r="C79">
         <f t="shared" si="15"/>
-        <v>0.12222222222222223</v>
+        <v>0.24444444444444446</v>
       </c>
       <c r="D79">
         <f t="shared" si="12"/>
-        <v>0.67777777777777781</v>
+        <v>0.97777777777777786</v>
       </c>
       <c r="E79">
         <f t="shared" si="7"/>
-        <v>16.666666666666664</v>
+        <v>12.777777777777779</v>
       </c>
       <c r="F79">
         <f t="shared" si="8"/>
-        <v>17.777777777777779</v>
+        <v>13.888888888888889</v>
       </c>
       <c r="G79">
         <f t="shared" si="9"/>
@@ -6022,7 +6022,7 @@
       </c>
       <c r="M79">
         <f t="shared" si="13"/>
-        <v>78</v>
+        <v>58.555555555555557</v>
       </c>
       <c r="N79">
         <v>-1</v>
@@ -6044,23 +6044,23 @@
       </c>
       <c r="B80">
         <f t="shared" si="14"/>
-        <v>39.415151515151514</v>
+        <v>23.657575757575756</v>
       </c>
       <c r="C80">
         <f t="shared" si="15"/>
-        <v>0.12121212121212122</v>
+        <v>0.24242424242424243</v>
       </c>
       <c r="D80">
         <f t="shared" si="12"/>
-        <v>0.66060606060606064</v>
+        <v>0.95151515151515165</v>
       </c>
       <c r="E80">
         <f t="shared" si="7"/>
-        <v>16.81818181818182</v>
+        <v>12.878787878787879</v>
       </c>
       <c r="F80">
         <f t="shared" si="8"/>
-        <v>17.878787878787879</v>
+        <v>13.939393939393939</v>
       </c>
       <c r="G80">
         <f t="shared" si="9"/>
@@ -6085,7 +6085,7 @@
       </c>
       <c r="M80">
         <f t="shared" si="13"/>
-        <v>79</v>
+        <v>59.303030303030297</v>
       </c>
       <c r="N80">
         <v>-1</v>
@@ -6107,23 +6107,23 @@
       </c>
       <c r="B81">
         <f t="shared" si="14"/>
-        <v>39.919191919191924</v>
+        <v>23.959595959595962</v>
       </c>
       <c r="C81">
         <f t="shared" si="15"/>
-        <v>0.1202020202020202</v>
+        <v>0.2404040404040404</v>
       </c>
       <c r="D81">
         <f t="shared" si="12"/>
-        <v>0.64343434343434347</v>
+        <v>0.92525252525252499</v>
       </c>
       <c r="E81">
         <f t="shared" si="7"/>
-        <v>16.969696969696969</v>
+        <v>12.979797979797979</v>
       </c>
       <c r="F81">
         <f t="shared" si="8"/>
-        <v>17.979797979797979</v>
+        <v>13.98989898989899</v>
       </c>
       <c r="G81">
         <f t="shared" si="9"/>
@@ -6148,7 +6148,7 @@
       </c>
       <c r="M81">
         <f t="shared" si="13"/>
-        <v>80</v>
+        <v>60.050505050505052</v>
       </c>
       <c r="N81">
         <v>-1</v>
@@ -6170,23 +6170,23 @@
       </c>
       <c r="B82">
         <f t="shared" si="14"/>
-        <v>40.42323232323232</v>
+        <v>24.261616161616161</v>
       </c>
       <c r="C82">
         <f t="shared" si="15"/>
-        <v>0.1191919191919192</v>
+        <v>0.23838383838383839</v>
       </c>
       <c r="D82">
         <f t="shared" si="12"/>
-        <v>0.6262626262626263</v>
+        <v>0.89898989898989878</v>
       </c>
       <c r="E82">
         <f t="shared" si="7"/>
-        <v>17.121212121212121</v>
+        <v>13.080808080808081</v>
       </c>
       <c r="F82">
         <f t="shared" si="8"/>
-        <v>18.080808080808083</v>
+        <v>14.040404040404042</v>
       </c>
       <c r="G82">
         <f t="shared" si="9"/>
@@ -6211,7 +6211,7 @@
       </c>
       <c r="M82">
         <f t="shared" si="13"/>
-        <v>81</v>
+        <v>60.797979797979799</v>
       </c>
       <c r="N82">
         <v>-1</v>
@@ -6233,23 +6233,23 @@
       </c>
       <c r="B83">
         <f t="shared" si="14"/>
-        <v>40.927272727272729</v>
+        <v>24.563636363636366</v>
       </c>
       <c r="C83">
         <f t="shared" si="15"/>
-        <v>0.11818181818181818</v>
+        <v>0.23636363636363636</v>
       </c>
       <c r="D83">
         <f t="shared" si="12"/>
-        <v>0.60909090909090913</v>
+        <v>0.87272727272727257</v>
       </c>
       <c r="E83">
         <f t="shared" ref="E83:E100" si="16">(E$2+((SUM($A83-1)/SUM($A$101-1))*(SUM(E$101-E$2))))</f>
-        <v>17.272727272727273</v>
+        <v>13.181818181818182</v>
       </c>
       <c r="F83">
         <f t="shared" ref="F83:F100" si="17">(F$2+((SUM($A83-1)/SUM($A$101-1))*(SUM(F$101-F$2))))</f>
-        <v>18.18181818181818</v>
+        <v>14.09090909090909</v>
       </c>
       <c r="G83">
         <f t="shared" ref="G83:H100" si="18">(G$2+((SUM($A83-1)/SUM($A$101-1))*(SUM(G$101-G$2))))</f>
@@ -6274,7 +6274,7 @@
       </c>
       <c r="M83">
         <f t="shared" si="13"/>
-        <v>82</v>
+        <v>61.545454545454547</v>
       </c>
       <c r="N83">
         <v>-1</v>
@@ -6296,23 +6296,23 @@
       </c>
       <c r="B84">
         <f t="shared" si="14"/>
-        <v>41.431313131313132</v>
+        <v>24.865656565656565</v>
       </c>
       <c r="C84">
         <f t="shared" si="15"/>
-        <v>0.11717171717171718</v>
+        <v>0.23434343434343435</v>
       </c>
       <c r="D84">
         <f t="shared" si="12"/>
-        <v>0.59191919191919196</v>
+        <v>0.84646464646464636</v>
       </c>
       <c r="E84">
         <f t="shared" si="16"/>
-        <v>17.424242424242422</v>
+        <v>13.282828282828284</v>
       </c>
       <c r="F84">
         <f t="shared" si="17"/>
-        <v>18.282828282828284</v>
+        <v>14.141414141414142</v>
       </c>
       <c r="G84">
         <f t="shared" si="18"/>
@@ -6337,7 +6337,7 @@
       </c>
       <c r="M84">
         <f t="shared" si="13"/>
-        <v>83</v>
+        <v>62.292929292929294</v>
       </c>
       <c r="N84">
         <v>-1</v>
@@ -6359,23 +6359,23 @@
       </c>
       <c r="B85">
         <f t="shared" si="14"/>
-        <v>41.935353535353535</v>
+        <v>25.167676767676767</v>
       </c>
       <c r="C85">
         <f t="shared" si="15"/>
-        <v>0.11616161616161617</v>
+        <v>0.23232323232323235</v>
       </c>
       <c r="D85">
         <f t="shared" si="12"/>
-        <v>0.57474747474747478</v>
+        <v>0.82020202020202015</v>
       </c>
       <c r="E85">
         <f t="shared" si="16"/>
-        <v>17.575757575757574</v>
+        <v>13.383838383838384</v>
       </c>
       <c r="F85">
         <f t="shared" si="17"/>
-        <v>18.383838383838384</v>
+        <v>14.191919191919192</v>
       </c>
       <c r="G85">
         <f t="shared" si="18"/>
@@ -6400,7 +6400,7 @@
       </c>
       <c r="M85">
         <f t="shared" si="13"/>
-        <v>84</v>
+        <v>63.040404040404034</v>
       </c>
       <c r="N85">
         <v>-1</v>
@@ -6422,23 +6422,23 @@
       </c>
       <c r="B86">
         <f t="shared" si="14"/>
-        <v>42.439393939393938</v>
+        <v>25.469696969696972</v>
       </c>
       <c r="C86">
         <f t="shared" si="15"/>
-        <v>0.11515151515151516</v>
+        <v>0.23030303030303031</v>
       </c>
       <c r="D86">
         <f t="shared" si="12"/>
-        <v>0.55757575757575761</v>
+        <v>0.79393939393939394</v>
       </c>
       <c r="E86">
         <f t="shared" si="16"/>
-        <v>17.727272727272727</v>
+        <v>13.484848484848484</v>
       </c>
       <c r="F86">
         <f t="shared" si="17"/>
-        <v>18.484848484848484</v>
+        <v>14.242424242424242</v>
       </c>
       <c r="G86">
         <f t="shared" si="18"/>
@@ -6463,7 +6463,7 @@
       </c>
       <c r="M86">
         <f t="shared" si="13"/>
-        <v>85</v>
+        <v>63.787878787878789</v>
       </c>
       <c r="N86">
         <v>-1</v>
@@ -6485,23 +6485,23 @@
       </c>
       <c r="B87">
         <f t="shared" si="14"/>
-        <v>42.94343434343434</v>
+        <v>25.771717171717171</v>
       </c>
       <c r="C87">
         <f t="shared" si="15"/>
-        <v>0.11414141414141415</v>
+        <v>0.22828282828282831</v>
       </c>
       <c r="D87">
         <f t="shared" si="12"/>
-        <v>0.54040404040404044</v>
+        <v>0.76767676767676774</v>
       </c>
       <c r="E87">
         <f t="shared" si="16"/>
-        <v>17.878787878787879</v>
+        <v>13.585858585858585</v>
       </c>
       <c r="F87">
         <f t="shared" si="17"/>
-        <v>18.585858585858585</v>
+        <v>14.292929292929292</v>
       </c>
       <c r="G87">
         <f t="shared" si="18"/>
@@ -6526,7 +6526,7 @@
       </c>
       <c r="M87">
         <f t="shared" si="13"/>
-        <v>86</v>
+        <v>64.535353535353536</v>
       </c>
       <c r="N87">
         <v>-1</v>
@@ -6548,23 +6548,23 @@
       </c>
       <c r="B88">
         <f t="shared" si="14"/>
-        <v>43.44747474747475</v>
+        <v>26.073737373737377</v>
       </c>
       <c r="C88">
         <f t="shared" si="15"/>
-        <v>0.11313131313131314</v>
+        <v>0.22626262626262628</v>
       </c>
       <c r="D88">
         <f t="shared" si="12"/>
-        <v>0.52323232323232327</v>
+        <v>0.74141414141414108</v>
       </c>
       <c r="E88">
         <f t="shared" si="16"/>
-        <v>18.030303030303031</v>
+        <v>13.686868686868687</v>
       </c>
       <c r="F88">
         <f t="shared" si="17"/>
-        <v>18.686868686868685</v>
+        <v>14.343434343434343</v>
       </c>
       <c r="G88">
         <f t="shared" si="18"/>
@@ -6589,7 +6589,7 @@
       </c>
       <c r="M88">
         <f t="shared" si="13"/>
-        <v>87</v>
+        <v>65.282828282828291</v>
       </c>
       <c r="N88">
         <v>-1</v>
@@ -6611,23 +6611,23 @@
       </c>
       <c r="B89">
         <f t="shared" si="14"/>
-        <v>43.951515151515153</v>
+        <v>26.375757575757575</v>
       </c>
       <c r="C89">
         <f t="shared" si="15"/>
-        <v>0.11212121212121212</v>
+        <v>0.22424242424242424</v>
       </c>
       <c r="D89">
         <f t="shared" si="12"/>
-        <v>0.5060606060606061</v>
+        <v>0.71515151515151487</v>
       </c>
       <c r="E89">
         <f t="shared" si="16"/>
-        <v>18.18181818181818</v>
+        <v>13.787878787878787</v>
       </c>
       <c r="F89">
         <f t="shared" si="17"/>
-        <v>18.787878787878789</v>
+        <v>14.393939393939394</v>
       </c>
       <c r="G89">
         <f t="shared" si="18"/>
@@ -6652,7 +6652,7 @@
       </c>
       <c r="M89">
         <f t="shared" si="13"/>
-        <v>88</v>
+        <v>66.030303030303031</v>
       </c>
       <c r="N89">
         <v>-1</v>
@@ -6674,23 +6674,23 @@
       </c>
       <c r="B90">
         <f t="shared" si="14"/>
-        <v>44.455555555555556</v>
+        <v>26.677777777777777</v>
       </c>
       <c r="C90">
         <f t="shared" si="15"/>
-        <v>0.11111111111111112</v>
+        <v>0.22222222222222224</v>
       </c>
       <c r="D90">
         <f t="shared" si="12"/>
-        <v>0.48888888888888893</v>
+        <v>0.68888888888888911</v>
       </c>
       <c r="E90">
         <f t="shared" si="16"/>
-        <v>18.333333333333332</v>
+        <v>13.888888888888889</v>
       </c>
       <c r="F90">
         <f t="shared" si="17"/>
-        <v>18.888888888888889</v>
+        <v>14.444444444444445</v>
       </c>
       <c r="G90">
         <f t="shared" si="18"/>
@@ -6715,7 +6715,7 @@
       </c>
       <c r="M90">
         <f t="shared" si="13"/>
-        <v>89</v>
+        <v>66.777777777777771</v>
       </c>
       <c r="N90">
         <v>-1</v>
@@ -6737,23 +6737,23 @@
       </c>
       <c r="B91">
         <f t="shared" si="14"/>
-        <v>44.959595959595958</v>
+        <v>26.979797979797979</v>
       </c>
       <c r="C91">
         <f t="shared" si="15"/>
-        <v>0.1101010101010101</v>
+        <v>0.2202020202020202</v>
       </c>
       <c r="D91">
         <f t="shared" si="12"/>
-        <v>0.47171717171717176</v>
+        <v>0.66262626262626245</v>
       </c>
       <c r="E91">
         <f t="shared" si="16"/>
-        <v>18.484848484848484</v>
+        <v>13.98989898989899</v>
       </c>
       <c r="F91">
         <f t="shared" si="17"/>
-        <v>18.98989898989899</v>
+        <v>14.494949494949495</v>
       </c>
       <c r="G91">
         <f t="shared" si="18"/>
@@ -6778,7 +6778,7 @@
       </c>
       <c r="M91">
         <f t="shared" si="13"/>
-        <v>90</v>
+        <v>67.525252525252526</v>
       </c>
       <c r="N91">
         <v>-1</v>
@@ -6800,23 +6800,23 @@
       </c>
       <c r="B92">
         <f t="shared" si="14"/>
-        <v>45.463636363636361</v>
+        <v>27.281818181818181</v>
       </c>
       <c r="C92">
         <f t="shared" si="15"/>
-        <v>0.1090909090909091</v>
+        <v>0.2181818181818182</v>
       </c>
       <c r="D92">
         <f t="shared" si="12"/>
-        <v>0.45454545454545459</v>
+        <v>0.63636363636363624</v>
       </c>
       <c r="E92">
         <f t="shared" si="16"/>
-        <v>18.636363636363637</v>
+        <v>14.09090909090909</v>
       </c>
       <c r="F92">
         <f t="shared" si="17"/>
-        <v>19.09090909090909</v>
+        <v>14.545454545454545</v>
       </c>
       <c r="G92">
         <f t="shared" si="18"/>
@@ -6841,7 +6841,7 @@
       </c>
       <c r="M92">
         <f t="shared" si="13"/>
-        <v>91</v>
+        <v>68.272727272727266</v>
       </c>
       <c r="N92">
         <v>-1</v>
@@ -6863,23 +6863,23 @@
       </c>
       <c r="B93">
         <f t="shared" si="14"/>
-        <v>45.967676767676771</v>
+        <v>27.583838383838383</v>
       </c>
       <c r="C93">
         <f t="shared" si="15"/>
-        <v>0.10808080808080808</v>
+        <v>0.21616161616161617</v>
       </c>
       <c r="D93">
         <f t="shared" si="12"/>
-        <v>0.43737373737373741</v>
+        <v>0.61010101010101003</v>
       </c>
       <c r="E93">
         <f t="shared" si="16"/>
-        <v>18.787878787878789</v>
+        <v>14.191919191919192</v>
       </c>
       <c r="F93">
         <f t="shared" si="17"/>
-        <v>19.19191919191919</v>
+        <v>14.595959595959595</v>
       </c>
       <c r="G93">
         <f t="shared" si="18"/>
@@ -6904,7 +6904,7 @@
       </c>
       <c r="M93">
         <f t="shared" si="13"/>
-        <v>92</v>
+        <v>69.020202020202021</v>
       </c>
       <c r="N93">
         <v>-1</v>
@@ -6926,23 +6926,23 @@
       </c>
       <c r="B94">
         <f t="shared" si="14"/>
-        <v>46.471717171717174</v>
+        <v>27.885858585858585</v>
       </c>
       <c r="C94">
         <f t="shared" si="15"/>
-        <v>0.10707070707070708</v>
+        <v>0.21414141414141416</v>
       </c>
       <c r="D94">
         <f t="shared" si="12"/>
-        <v>0.42020202020202024</v>
+        <v>0.58383838383838382</v>
       </c>
       <c r="E94">
         <f t="shared" si="16"/>
-        <v>18.939393939393938</v>
+        <v>14.292929292929292</v>
       </c>
       <c r="F94">
         <f t="shared" si="17"/>
-        <v>19.292929292929294</v>
+        <v>14.646464646464647</v>
       </c>
       <c r="G94">
         <f t="shared" si="18"/>
@@ -6967,7 +6967,7 @@
       </c>
       <c r="M94">
         <f t="shared" si="13"/>
-        <v>93</v>
+        <v>69.767676767676761</v>
       </c>
       <c r="N94">
         <v>-1</v>
@@ -6989,23 +6989,23 @@
       </c>
       <c r="B95">
         <f t="shared" si="14"/>
-        <v>46.975757575757576</v>
+        <v>28.187878787878791</v>
       </c>
       <c r="C95">
         <f t="shared" si="15"/>
-        <v>0.10606060606060606</v>
+        <v>0.21212121212121213</v>
       </c>
       <c r="D95">
         <f t="shared" si="12"/>
-        <v>0.40303030303030307</v>
+        <v>0.55757575757575717</v>
       </c>
       <c r="E95">
         <f t="shared" si="16"/>
-        <v>19.090909090909093</v>
+        <v>14.393939393939394</v>
       </c>
       <c r="F95">
         <f t="shared" si="17"/>
-        <v>19.393939393939394</v>
+        <v>14.696969696969697</v>
       </c>
       <c r="G95">
         <f t="shared" si="18"/>
@@ -7030,7 +7030,7 @@
       </c>
       <c r="M95">
         <f t="shared" si="13"/>
-        <v>94</v>
+        <v>70.515151515151516</v>
       </c>
       <c r="N95">
         <v>-1</v>
@@ -7052,23 +7052,23 @@
       </c>
       <c r="B96">
         <f t="shared" si="14"/>
-        <v>47.479797979797979</v>
+        <v>28.48989898989899</v>
       </c>
       <c r="C96">
         <f t="shared" si="15"/>
-        <v>0.10505050505050506</v>
+        <v>0.21010101010101012</v>
       </c>
       <c r="D96">
         <f t="shared" si="12"/>
-        <v>0.3858585858585859</v>
+        <v>0.5313131313131314</v>
       </c>
       <c r="E96">
         <f t="shared" si="16"/>
-        <v>19.242424242424242</v>
+        <v>14.494949494949495</v>
       </c>
       <c r="F96">
         <f t="shared" si="17"/>
-        <v>19.494949494949495</v>
+        <v>14.747474747474747</v>
       </c>
       <c r="G96">
         <f t="shared" si="18"/>
@@ -7093,7 +7093,7 @@
       </c>
       <c r="M96">
         <f t="shared" si="13"/>
-        <v>95</v>
+        <v>71.26262626262627</v>
       </c>
       <c r="N96">
         <v>-1</v>
@@ -7115,23 +7115,23 @@
       </c>
       <c r="B97">
         <f t="shared" si="14"/>
-        <v>47.983838383838382</v>
+        <v>28.791919191919192</v>
       </c>
       <c r="C97">
         <f t="shared" si="15"/>
-        <v>0.10404040404040404</v>
+        <v>0.20808080808080809</v>
       </c>
       <c r="D97">
         <f t="shared" si="12"/>
-        <v>0.36868686868686873</v>
+        <v>0.50505050505050519</v>
       </c>
       <c r="E97">
         <f t="shared" si="16"/>
-        <v>19.393939393939391</v>
+        <v>14.595959595959595</v>
       </c>
       <c r="F97">
         <f t="shared" si="17"/>
-        <v>19.595959595959595</v>
+        <v>14.797979797979798</v>
       </c>
       <c r="G97">
         <f t="shared" si="18"/>
@@ -7156,7 +7156,7 @@
       </c>
       <c r="M97">
         <f t="shared" si="13"/>
-        <v>96</v>
+        <v>72.01010101010101</v>
       </c>
       <c r="N97">
         <v>-1</v>
@@ -7178,23 +7178,23 @@
       </c>
       <c r="B98">
         <f t="shared" si="14"/>
-        <v>48.487878787878792</v>
+        <v>29.093939393939394</v>
       </c>
       <c r="C98">
         <f t="shared" si="15"/>
-        <v>0.10303030303030303</v>
+        <v>0.20606060606060606</v>
       </c>
       <c r="D98">
         <f t="shared" si="12"/>
-        <v>0.35151515151515156</v>
+        <v>0.47878787878787854</v>
       </c>
       <c r="E98">
         <f t="shared" si="16"/>
-        <v>19.545454545454547</v>
+        <v>14.696969696969697</v>
       </c>
       <c r="F98">
         <f t="shared" si="17"/>
-        <v>19.696969696969695</v>
+        <v>14.848484848484848</v>
       </c>
       <c r="G98">
         <f t="shared" si="18"/>
@@ -7219,7 +7219,7 @@
       </c>
       <c r="M98">
         <f t="shared" si="13"/>
-        <v>97</v>
+        <v>72.757575757575765</v>
       </c>
       <c r="N98">
         <v>-1</v>
@@ -7241,23 +7241,23 @@
       </c>
       <c r="B99">
         <f t="shared" si="14"/>
-        <v>48.991919191919195</v>
+        <v>29.395959595959596</v>
       </c>
       <c r="C99">
         <f t="shared" si="15"/>
-        <v>0.10202020202020202</v>
+        <v>0.20404040404040405</v>
       </c>
       <c r="D99">
         <f t="shared" si="12"/>
-        <v>0.33434343434343439</v>
+        <v>0.45252525252525233</v>
       </c>
       <c r="E99">
         <f t="shared" si="16"/>
-        <v>19.696969696969695</v>
+        <v>14.797979797979798</v>
       </c>
       <c r="F99">
         <f t="shared" si="17"/>
-        <v>19.797979797979799</v>
+        <v>14.8989898989899</v>
       </c>
       <c r="G99">
         <f t="shared" si="18"/>
@@ -7282,7 +7282,7 @@
       </c>
       <c r="M99">
         <f t="shared" si="13"/>
-        <v>98</v>
+        <v>73.505050505050505</v>
       </c>
       <c r="N99">
         <v>-1</v>
@@ -7304,23 +7304,23 @@
       </c>
       <c r="B100">
         <f t="shared" si="14"/>
-        <v>49.495959595959597</v>
+        <v>29.697979797979798</v>
       </c>
       <c r="C100">
         <f t="shared" si="15"/>
-        <v>0.10101010101010101</v>
+        <v>0.20202020202020202</v>
       </c>
       <c r="D100">
         <f t="shared" si="12"/>
-        <v>0.31717171717171722</v>
+        <v>0.42626262626262612</v>
       </c>
       <c r="E100">
         <f t="shared" si="16"/>
-        <v>19.848484848484851</v>
+        <v>14.8989898989899</v>
       </c>
       <c r="F100">
         <f t="shared" si="17"/>
-        <v>19.8989898989899</v>
+        <v>14.94949494949495</v>
       </c>
       <c r="G100">
         <f t="shared" si="18"/>
@@ -7345,7 +7345,7 @@
       </c>
       <c r="M100">
         <f t="shared" si="13"/>
-        <v>99</v>
+        <v>74.25252525252526</v>
       </c>
       <c r="N100">
         <v>-1</v>
@@ -7366,19 +7366,19 @@
         <v>100</v>
       </c>
       <c r="B101" s="1">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C101" s="1">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="D101" s="1">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="E101" s="1">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F101" s="1">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G101" s="1">
         <v>100</v>
@@ -7399,7 +7399,7 @@
         <v>-1</v>
       </c>
       <c r="M101" s="1">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="N101" s="1">
         <v>-1</v>

</xml_diff>

<commit_message>
set up 10 new enemy paths improved enemy firing rate & distance
</commit_message>
<xml_diff>
--- a/RotoShootUnityProject/Assets/Resources/mySheet.xlsx
+++ b/RotoShootUnityProject/Assets/Resources/mySheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\UnityProjects\RotoShoot\RotoShootUnityProject\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD170AD-3158-47B5-BEB3-83FA615FD93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867525FF-592E-48EA-A2BF-E05692C21792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="37605" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25490" yWindow="90" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mySheet (4)" sheetId="4" r:id="rId1"/>
@@ -1067,7 +1067,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,7 +1078,7 @@
     <col min="6" max="6" width="19.85546875" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="17" max="17" width="21.7109375" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -1178,7 +1178,7 @@
         <v>-1</v>
       </c>
       <c r="O2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P2" s="1">
         <v>-1</v>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="O3">
         <f t="shared" si="2"/>
-        <v>3.0101010101010104</v>
+        <v>4</v>
       </c>
       <c r="P3">
         <v>-1</v>
@@ -1304,7 +1304,7 @@
       </c>
       <c r="O4">
         <f t="shared" si="2"/>
-        <v>5.0202020202020208</v>
+        <v>6</v>
       </c>
       <c r="P4">
         <v>-1</v>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="O5">
         <f t="shared" si="2"/>
-        <v>7.0303030303030303</v>
+        <v>8</v>
       </c>
       <c r="P5">
         <v>-1</v>
@@ -1430,7 +1430,7 @@
       </c>
       <c r="O6">
         <f t="shared" si="2"/>
-        <v>9.0404040404040416</v>
+        <v>10</v>
       </c>
       <c r="P6">
         <v>-1</v>
@@ -1493,7 +1493,7 @@
       </c>
       <c r="O7">
         <f t="shared" si="2"/>
-        <v>11.05050505050505</v>
+        <v>12</v>
       </c>
       <c r="P7">
         <v>-1</v>
@@ -1556,7 +1556,7 @@
       </c>
       <c r="O8">
         <f t="shared" si="2"/>
-        <v>13.060606060606061</v>
+        <v>14</v>
       </c>
       <c r="P8">
         <v>-1</v>
@@ -1619,7 +1619,7 @@
       </c>
       <c r="O9">
         <f t="shared" si="2"/>
-        <v>15.070707070707071</v>
+        <v>16</v>
       </c>
       <c r="P9">
         <v>-1</v>
@@ -1682,7 +1682,7 @@
       </c>
       <c r="O10">
         <f t="shared" si="2"/>
-        <v>17.080808080808083</v>
+        <v>18</v>
       </c>
       <c r="P10">
         <v>-1</v>
@@ -1745,7 +1745,7 @@
       </c>
       <c r="O11">
         <f t="shared" si="2"/>
-        <v>19.09090909090909</v>
+        <v>20</v>
       </c>
       <c r="P11">
         <v>-1</v>
@@ -1808,7 +1808,7 @@
       </c>
       <c r="O12">
         <f t="shared" si="2"/>
-        <v>21.1010101010101</v>
+        <v>22</v>
       </c>
       <c r="P12">
         <v>-1</v>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="O13">
         <f t="shared" si="2"/>
-        <v>23.111111111111111</v>
+        <v>24</v>
       </c>
       <c r="P13">
         <v>-1</v>
@@ -1934,7 +1934,7 @@
       </c>
       <c r="O14">
         <f t="shared" si="2"/>
-        <v>25.121212121212121</v>
+        <v>26</v>
       </c>
       <c r="P14">
         <v>-1</v>
@@ -1997,7 +1997,7 @@
       </c>
       <c r="O15">
         <f t="shared" si="2"/>
-        <v>27.131313131313135</v>
+        <v>28.000000000000004</v>
       </c>
       <c r="P15">
         <v>-1</v>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="O16">
         <f t="shared" si="2"/>
-        <v>29.141414141414142</v>
+        <v>30</v>
       </c>
       <c r="P16">
         <v>-1</v>
@@ -2123,7 +2123,7 @@
       </c>
       <c r="O17">
         <f t="shared" si="2"/>
-        <v>31.151515151515152</v>
+        <v>32</v>
       </c>
       <c r="P17">
         <v>-1</v>
@@ -2186,7 +2186,7 @@
       </c>
       <c r="O18">
         <f t="shared" si="2"/>
-        <v>33.161616161616166</v>
+        <v>34</v>
       </c>
       <c r="P18">
         <v>-1</v>
@@ -2249,7 +2249,7 @@
       </c>
       <c r="O19">
         <f t="shared" si="2"/>
-        <v>35.171717171717169</v>
+        <v>36</v>
       </c>
       <c r="P19">
         <v>-1</v>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="O20">
         <f t="shared" si="2"/>
-        <v>37.18181818181818</v>
+        <v>38</v>
       </c>
       <c r="P20">
         <v>-1</v>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="O21">
         <f t="shared" si="2"/>
-        <v>39.19191919191919</v>
+        <v>40</v>
       </c>
       <c r="P21">
         <v>-1</v>
@@ -2438,7 +2438,7 @@
       </c>
       <c r="O22">
         <f t="shared" si="2"/>
-        <v>41.202020202020201</v>
+        <v>42</v>
       </c>
       <c r="P22">
         <v>-1</v>
@@ -2501,7 +2501,7 @@
       </c>
       <c r="O23">
         <f t="shared" si="2"/>
-        <v>43.212121212121211</v>
+        <v>44</v>
       </c>
       <c r="P23">
         <v>-1</v>
@@ -2564,7 +2564,7 @@
       </c>
       <c r="O24">
         <f t="shared" si="2"/>
-        <v>45.222222222222221</v>
+        <v>46</v>
       </c>
       <c r="P24">
         <v>-1</v>
@@ -2627,7 +2627,7 @@
       </c>
       <c r="O25">
         <f t="shared" si="2"/>
-        <v>47.232323232323232</v>
+        <v>48</v>
       </c>
       <c r="P25">
         <v>-1</v>
@@ -2690,7 +2690,7 @@
       </c>
       <c r="O26">
         <f t="shared" si="2"/>
-        <v>49.242424242424242</v>
+        <v>50</v>
       </c>
       <c r="P26">
         <v>-1</v>
@@ -2753,7 +2753,7 @@
       </c>
       <c r="O27">
         <f t="shared" si="2"/>
-        <v>51.252525252525253</v>
+        <v>52</v>
       </c>
       <c r="P27">
         <v>-1</v>
@@ -2816,7 +2816,7 @@
       </c>
       <c r="O28">
         <f t="shared" si="2"/>
-        <v>53.26262626262627</v>
+        <v>54.000000000000007</v>
       </c>
       <c r="P28">
         <v>-1</v>
@@ -2879,7 +2879,7 @@
       </c>
       <c r="O29">
         <f t="shared" si="2"/>
-        <v>55.272727272727266</v>
+        <v>55.999999999999993</v>
       </c>
       <c r="P29">
         <v>-1</v>
@@ -2942,7 +2942,7 @@
       </c>
       <c r="O30">
         <f t="shared" si="2"/>
-        <v>57.282828282828284</v>
+        <v>58</v>
       </c>
       <c r="P30">
         <v>-1</v>
@@ -3005,7 +3005,7 @@
       </c>
       <c r="O31">
         <f t="shared" si="2"/>
-        <v>59.292929292929294</v>
+        <v>60</v>
       </c>
       <c r="P31">
         <v>-1</v>
@@ -3068,7 +3068,7 @@
       </c>
       <c r="O32">
         <f t="shared" si="2"/>
-        <v>61.303030303030305</v>
+        <v>62</v>
       </c>
       <c r="P32">
         <v>-1</v>
@@ -3131,7 +3131,7 @@
       </c>
       <c r="O33">
         <f t="shared" si="2"/>
-        <v>63.313131313131315</v>
+        <v>64</v>
       </c>
       <c r="P33">
         <v>-1</v>
@@ -3194,7 +3194,7 @@
       </c>
       <c r="O34">
         <f t="shared" si="2"/>
-        <v>65.323232323232332</v>
+        <v>66</v>
       </c>
       <c r="P34">
         <v>-1</v>
@@ -3257,7 +3257,7 @@
       </c>
       <c r="O35">
         <f t="shared" si="2"/>
-        <v>67.333333333333329</v>
+        <v>68</v>
       </c>
       <c r="P35">
         <v>-1</v>
@@ -3320,7 +3320,7 @@
       </c>
       <c r="O36">
         <f t="shared" si="2"/>
-        <v>69.343434343434339</v>
+        <v>70</v>
       </c>
       <c r="P36">
         <v>-1</v>
@@ -3383,7 +3383,7 @@
       </c>
       <c r="O37">
         <f t="shared" si="2"/>
-        <v>71.353535353535349</v>
+        <v>72</v>
       </c>
       <c r="P37">
         <v>-1</v>
@@ -3446,7 +3446,7 @@
       </c>
       <c r="O38">
         <f t="shared" si="2"/>
-        <v>73.36363636363636</v>
+        <v>74</v>
       </c>
       <c r="P38">
         <v>-1</v>
@@ -3509,7 +3509,7 @@
       </c>
       <c r="O39">
         <f t="shared" si="2"/>
-        <v>75.373737373737384</v>
+        <v>76</v>
       </c>
       <c r="P39">
         <v>-1</v>
@@ -3572,7 +3572,7 @@
       </c>
       <c r="O40">
         <f t="shared" si="2"/>
-        <v>77.383838383838381</v>
+        <v>78</v>
       </c>
       <c r="P40">
         <v>-1</v>
@@ -3635,7 +3635,7 @@
       </c>
       <c r="O41">
         <f t="shared" si="2"/>
-        <v>79.393939393939391</v>
+        <v>80</v>
       </c>
       <c r="P41">
         <v>-1</v>
@@ -3698,7 +3698,7 @@
       </c>
       <c r="O42">
         <f t="shared" si="2"/>
-        <v>81.404040404040401</v>
+        <v>82</v>
       </c>
       <c r="P42">
         <v>-1</v>
@@ -3761,7 +3761,7 @@
       </c>
       <c r="O43">
         <f t="shared" si="2"/>
-        <v>83.414141414141412</v>
+        <v>84</v>
       </c>
       <c r="P43">
         <v>-1</v>
@@ -3824,7 +3824,7 @@
       </c>
       <c r="O44">
         <f t="shared" si="2"/>
-        <v>85.424242424242422</v>
+        <v>86</v>
       </c>
       <c r="P44">
         <v>-1</v>
@@ -3887,7 +3887,7 @@
       </c>
       <c r="O45">
         <f t="shared" si="2"/>
-        <v>87.434343434343432</v>
+        <v>88</v>
       </c>
       <c r="P45">
         <v>-1</v>
@@ -3950,7 +3950,7 @@
       </c>
       <c r="O46">
         <f t="shared" si="2"/>
-        <v>89.444444444444443</v>
+        <v>90</v>
       </c>
       <c r="P46">
         <v>-1</v>
@@ -4013,7 +4013,7 @@
       </c>
       <c r="O47">
         <f t="shared" si="2"/>
-        <v>91.454545454545453</v>
+        <v>92</v>
       </c>
       <c r="P47">
         <v>-1</v>
@@ -4076,7 +4076,7 @@
       </c>
       <c r="O48">
         <f t="shared" si="2"/>
-        <v>93.464646464646464</v>
+        <v>94</v>
       </c>
       <c r="P48">
         <v>-1</v>
@@ -4139,7 +4139,7 @@
       </c>
       <c r="O49">
         <f t="shared" si="2"/>
-        <v>95.474747474747474</v>
+        <v>96</v>
       </c>
       <c r="P49">
         <v>-1</v>
@@ -4202,7 +4202,7 @@
       </c>
       <c r="O50">
         <f t="shared" si="2"/>
-        <v>97.484848484848484</v>
+        <v>98</v>
       </c>
       <c r="P50">
         <v>-1</v>
@@ -4265,7 +4265,7 @@
       </c>
       <c r="O51">
         <f t="shared" si="2"/>
-        <v>99.494949494949495</v>
+        <v>100</v>
       </c>
       <c r="P51">
         <v>-1</v>
@@ -4328,7 +4328,7 @@
       </c>
       <c r="O52">
         <f t="shared" si="2"/>
-        <v>101.50505050505051</v>
+        <v>102</v>
       </c>
       <c r="P52">
         <v>-1</v>
@@ -4391,7 +4391,7 @@
       </c>
       <c r="O53">
         <f t="shared" si="2"/>
-        <v>103.51515151515152</v>
+        <v>104</v>
       </c>
       <c r="P53">
         <v>-1</v>
@@ -4454,7 +4454,7 @@
       </c>
       <c r="O54">
         <f t="shared" si="2"/>
-        <v>105.52525252525254</v>
+        <v>106.00000000000001</v>
       </c>
       <c r="P54">
         <v>-1</v>
@@ -4517,7 +4517,7 @@
       </c>
       <c r="O55">
         <f t="shared" si="2"/>
-        <v>107.53535353535354</v>
+        <v>108</v>
       </c>
       <c r="P55">
         <v>-1</v>
@@ -4580,7 +4580,7 @@
       </c>
       <c r="O56">
         <f t="shared" si="2"/>
-        <v>109.54545454545453</v>
+        <v>109.99999999999999</v>
       </c>
       <c r="P56">
         <v>-1</v>
@@ -4643,7 +4643,7 @@
       </c>
       <c r="O57">
         <f t="shared" si="2"/>
-        <v>111.55555555555556</v>
+        <v>112</v>
       </c>
       <c r="P57">
         <v>-1</v>
@@ -4706,7 +4706,7 @@
       </c>
       <c r="O58">
         <f t="shared" si="2"/>
-        <v>113.56565656565657</v>
+        <v>114</v>
       </c>
       <c r="P58">
         <v>-1</v>
@@ -4769,7 +4769,7 @@
       </c>
       <c r="O59">
         <f t="shared" si="2"/>
-        <v>115.57575757575758</v>
+        <v>116.00000000000001</v>
       </c>
       <c r="P59">
         <v>-1</v>
@@ -4832,7 +4832,7 @@
       </c>
       <c r="O60">
         <f t="shared" si="2"/>
-        <v>117.58585858585859</v>
+        <v>118</v>
       </c>
       <c r="P60">
         <v>-1</v>
@@ -4895,7 +4895,7 @@
       </c>
       <c r="O61">
         <f t="shared" si="2"/>
-        <v>119.59595959595958</v>
+        <v>119.99999999999999</v>
       </c>
       <c r="P61">
         <v>-1</v>
@@ -4958,7 +4958,7 @@
       </c>
       <c r="O62">
         <f t="shared" si="2"/>
-        <v>121.60606060606061</v>
+        <v>122</v>
       </c>
       <c r="P62">
         <v>-1</v>
@@ -5021,7 +5021,7 @@
       </c>
       <c r="O63">
         <f t="shared" si="2"/>
-        <v>123.61616161616161</v>
+        <v>124</v>
       </c>
       <c r="P63">
         <v>-1</v>
@@ -5084,7 +5084,7 @@
       </c>
       <c r="O64">
         <f t="shared" si="2"/>
-        <v>125.62626262626263</v>
+        <v>126</v>
       </c>
       <c r="P64">
         <v>-1</v>
@@ -5147,7 +5147,7 @@
       </c>
       <c r="O65">
         <f t="shared" si="2"/>
-        <v>127.63636363636364</v>
+        <v>128</v>
       </c>
       <c r="P65">
         <v>-1</v>
@@ -5210,7 +5210,7 @@
       </c>
       <c r="O66">
         <f t="shared" si="2"/>
-        <v>129.64646464646466</v>
+        <v>130</v>
       </c>
       <c r="P66">
         <v>-1</v>
@@ -5273,7 +5273,7 @@
       </c>
       <c r="O67">
         <f t="shared" si="13"/>
-        <v>131.65656565656565</v>
+        <v>132</v>
       </c>
       <c r="P67">
         <v>-1</v>
@@ -5336,7 +5336,7 @@
       </c>
       <c r="O68">
         <f t="shared" si="13"/>
-        <v>133.66666666666666</v>
+        <v>134</v>
       </c>
       <c r="P68">
         <v>-1</v>
@@ -5399,7 +5399,7 @@
       </c>
       <c r="O69">
         <f t="shared" si="13"/>
-        <v>135.6767676767677</v>
+        <v>136</v>
       </c>
       <c r="P69">
         <v>-1</v>
@@ -5462,7 +5462,7 @@
       </c>
       <c r="O70">
         <f t="shared" si="13"/>
-        <v>137.68686868686868</v>
+        <v>138</v>
       </c>
       <c r="P70">
         <v>-1</v>
@@ -5525,7 +5525,7 @@
       </c>
       <c r="O71">
         <f t="shared" si="13"/>
-        <v>139.69696969696972</v>
+        <v>140</v>
       </c>
       <c r="P71">
         <v>-1</v>
@@ -5588,7 +5588,7 @@
       </c>
       <c r="O72">
         <f t="shared" si="13"/>
-        <v>141.7070707070707</v>
+        <v>142</v>
       </c>
       <c r="P72">
         <v>-1</v>
@@ -5651,7 +5651,7 @@
       </c>
       <c r="O73">
         <f t="shared" si="13"/>
-        <v>143.71717171717171</v>
+        <v>144</v>
       </c>
       <c r="P73">
         <v>-1</v>
@@ -5714,7 +5714,7 @@
       </c>
       <c r="O74">
         <f t="shared" si="13"/>
-        <v>145.72727272727272</v>
+        <v>146</v>
       </c>
       <c r="P74">
         <v>-1</v>
@@ -5777,7 +5777,7 @@
       </c>
       <c r="O75">
         <f t="shared" si="13"/>
-        <v>147.73737373737373</v>
+        <v>148</v>
       </c>
       <c r="P75">
         <v>-1</v>
@@ -5840,7 +5840,7 @@
       </c>
       <c r="O76">
         <f t="shared" si="13"/>
-        <v>149.74747474747477</v>
+        <v>150</v>
       </c>
       <c r="P76">
         <v>-1</v>
@@ -5903,7 +5903,7 @@
       </c>
       <c r="O77">
         <f t="shared" si="13"/>
-        <v>151.75757575757575</v>
+        <v>152</v>
       </c>
       <c r="P77">
         <v>-1</v>
@@ -5966,7 +5966,7 @@
       </c>
       <c r="O78">
         <f t="shared" si="13"/>
-        <v>153.76767676767676</v>
+        <v>154</v>
       </c>
       <c r="P78">
         <v>-1</v>
@@ -6029,7 +6029,7 @@
       </c>
       <c r="O79">
         <f t="shared" si="13"/>
-        <v>155.77777777777777</v>
+        <v>156</v>
       </c>
       <c r="P79">
         <v>-1</v>
@@ -6092,7 +6092,7 @@
       </c>
       <c r="O80">
         <f t="shared" si="13"/>
-        <v>157.78787878787878</v>
+        <v>158</v>
       </c>
       <c r="P80">
         <v>-1</v>
@@ -6155,7 +6155,7 @@
       </c>
       <c r="O81">
         <f t="shared" si="13"/>
-        <v>159.79797979797979</v>
+        <v>160</v>
       </c>
       <c r="P81">
         <v>-1</v>
@@ -6218,7 +6218,7 @@
       </c>
       <c r="O82">
         <f t="shared" si="13"/>
-        <v>161.8080808080808</v>
+        <v>162</v>
       </c>
       <c r="P82">
         <v>-1</v>
@@ -6281,7 +6281,7 @@
       </c>
       <c r="O83">
         <f t="shared" si="13"/>
-        <v>163.81818181818184</v>
+        <v>164</v>
       </c>
       <c r="P83">
         <v>-1</v>
@@ -6344,7 +6344,7 @@
       </c>
       <c r="O84">
         <f t="shared" si="13"/>
-        <v>165.82828282828282</v>
+        <v>166</v>
       </c>
       <c r="P84">
         <v>-1</v>
@@ -6407,7 +6407,7 @@
       </c>
       <c r="O85">
         <f t="shared" si="13"/>
-        <v>167.83838383838383</v>
+        <v>168</v>
       </c>
       <c r="P85">
         <v>-1</v>
@@ -6470,7 +6470,7 @@
       </c>
       <c r="O86">
         <f t="shared" si="13"/>
-        <v>169.84848484848484</v>
+        <v>170</v>
       </c>
       <c r="P86">
         <v>-1</v>
@@ -6533,7 +6533,7 @@
       </c>
       <c r="O87">
         <f t="shared" si="13"/>
-        <v>171.85858585858585</v>
+        <v>172</v>
       </c>
       <c r="P87">
         <v>-1</v>
@@ -6596,7 +6596,7 @@
       </c>
       <c r="O88">
         <f t="shared" si="13"/>
-        <v>173.86868686868686</v>
+        <v>174</v>
       </c>
       <c r="P88">
         <v>-1</v>
@@ -6659,7 +6659,7 @@
       </c>
       <c r="O89">
         <f t="shared" si="13"/>
-        <v>175.87878787878788</v>
+        <v>176</v>
       </c>
       <c r="P89">
         <v>-1</v>
@@ -6722,7 +6722,7 @@
       </c>
       <c r="O90">
         <f t="shared" si="13"/>
-        <v>177.88888888888889</v>
+        <v>178</v>
       </c>
       <c r="P90">
         <v>-1</v>
@@ -6785,7 +6785,7 @@
       </c>
       <c r="O91">
         <f t="shared" si="13"/>
-        <v>179.8989898989899</v>
+        <v>180</v>
       </c>
       <c r="P91">
         <v>-1</v>
@@ -6848,7 +6848,7 @@
       </c>
       <c r="O92">
         <f t="shared" si="13"/>
-        <v>181.90909090909091</v>
+        <v>182</v>
       </c>
       <c r="P92">
         <v>-1</v>
@@ -6911,7 +6911,7 @@
       </c>
       <c r="O93">
         <f t="shared" si="13"/>
-        <v>183.91919191919192</v>
+        <v>184</v>
       </c>
       <c r="P93">
         <v>-1</v>
@@ -6974,7 +6974,7 @@
       </c>
       <c r="O94">
         <f t="shared" si="13"/>
-        <v>185.92929292929293</v>
+        <v>186</v>
       </c>
       <c r="P94">
         <v>-1</v>
@@ -7037,7 +7037,7 @@
       </c>
       <c r="O95">
         <f t="shared" si="13"/>
-        <v>187.93939393939394</v>
+        <v>188</v>
       </c>
       <c r="P95">
         <v>-1</v>
@@ -7100,7 +7100,7 @@
       </c>
       <c r="O96">
         <f t="shared" si="13"/>
-        <v>189.94949494949495</v>
+        <v>190</v>
       </c>
       <c r="P96">
         <v>-1</v>
@@ -7163,7 +7163,7 @@
       </c>
       <c r="O97">
         <f t="shared" si="13"/>
-        <v>191.95959595959596</v>
+        <v>192</v>
       </c>
       <c r="P97">
         <v>-1</v>
@@ -7226,7 +7226,7 @@
       </c>
       <c r="O98">
         <f t="shared" si="13"/>
-        <v>193.96969696969697</v>
+        <v>194</v>
       </c>
       <c r="P98">
         <v>-1</v>
@@ -7289,7 +7289,7 @@
       </c>
       <c r="O99">
         <f t="shared" si="13"/>
-        <v>195.97979797979798</v>
+        <v>196</v>
       </c>
       <c r="P99">
         <v>-1</v>
@@ -7352,7 +7352,7 @@
       </c>
       <c r="O100">
         <f t="shared" si="13"/>
-        <v>197.98989898989899</v>
+        <v>198</v>
       </c>
       <c r="P100">
         <v>-1</v>

</xml_diff>

<commit_message>
LevelSetups for 006 and 007
</commit_message>
<xml_diff>
--- a/RotoShootUnityProject/Assets/Resources/mySheet.xlsx
+++ b/RotoShootUnityProject/Assets/Resources/mySheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\UnityProjects\RotoShoot\RotoShootUnityProject\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867525FF-592E-48EA-A2BF-E05692C21792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37745BC-3107-411E-892C-D2C6E793A975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25490" yWindow="90" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1067,7 +1067,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,7 +1139,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
       <c r="C2" s="1">
         <v>0.4</v>
@@ -1193,7 +1193,7 @@
       </c>
       <c r="B3">
         <f>(B$2+((SUM($A3-1)/SUM($A$101-1))*(SUM(B$101-B$2))))</f>
-        <v>0.40202020202020206</v>
+        <v>0.24341414141414142</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:H18" si="0">(C$2+((SUM($A3-1)/SUM($A$101-1))*(SUM(C$101-C$2))))</f>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="B4">
         <f t="shared" ref="B4:B5" si="3">(B$2+((SUM($A4-1)/SUM($A$101-1))*(SUM(B$101-B$2))))</f>
-        <v>0.70404040404040402</v>
+        <v>0.48582828282828283</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
@@ -1319,7 +1319,7 @@
       </c>
       <c r="B5">
         <f t="shared" si="3"/>
-        <v>1.0060606060606061</v>
+        <v>0.72824242424242425</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
@@ -1382,7 +1382,7 @@
       </c>
       <c r="B6">
         <f t="shared" ref="B6" si="4">(B$2+((SUM(A6-1)/SUM(A$101-1))*(SUM(B$101-B$2))))</f>
-        <v>1.3080808080808082</v>
+        <v>0.97065656565656566</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
@@ -1445,7 +1445,7 @@
       </c>
       <c r="B7">
         <f t="shared" ref="B7:B67" si="5">(B$2+((SUM(A7-1)/SUM(A$101-1))*(SUM(B$101-B$2))))</f>
-        <v>1.61010101010101</v>
+        <v>1.213070707070707</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
@@ -1508,7 +1508,7 @@
       </c>
       <c r="B8">
         <f t="shared" si="5"/>
-        <v>1.9121212121212121</v>
+        <v>1.4554848484848484</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="B9">
         <f t="shared" si="5"/>
-        <v>2.2141414141414142</v>
+        <v>1.6978989898989896</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
@@ -1634,7 +1634,7 @@
       </c>
       <c r="B10">
         <f t="shared" si="5"/>
-        <v>2.5161616161616163</v>
+        <v>1.9403131313131312</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
@@ -1697,7 +1697,7 @@
       </c>
       <c r="B11">
         <f t="shared" si="5"/>
-        <v>2.8181818181818183</v>
+        <v>2.1827272727272726</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
@@ -1760,7 +1760,7 @@
       </c>
       <c r="B12">
         <f t="shared" si="5"/>
-        <v>3.12020202020202</v>
+        <v>2.425141414141414</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
@@ -1823,7 +1823,7 @@
       </c>
       <c r="B13">
         <f t="shared" si="5"/>
-        <v>3.4222222222222221</v>
+        <v>2.667555555555555</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
@@ -1886,7 +1886,7 @@
       </c>
       <c r="B14">
         <f t="shared" si="5"/>
-        <v>3.7242424242424241</v>
+        <v>2.9099696969696969</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="B15">
         <f t="shared" si="5"/>
-        <v>4.0262626262626267</v>
+        <v>3.1523838383838383</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
@@ -2012,7 +2012,7 @@
       </c>
       <c r="B16">
         <f t="shared" si="5"/>
-        <v>4.3282828282828278</v>
+        <v>3.3947979797979793</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
@@ -2075,7 +2075,7 @@
       </c>
       <c r="B17">
         <f t="shared" si="5"/>
-        <v>4.6303030303030299</v>
+        <v>3.6372121212121211</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
@@ -2138,7 +2138,7 @@
       </c>
       <c r="B18">
         <f t="shared" si="5"/>
-        <v>4.932323232323232</v>
+        <v>3.8796262626262625</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
@@ -2201,7 +2201,7 @@
       </c>
       <c r="B19">
         <f t="shared" si="5"/>
-        <v>5.2343434343434332</v>
+        <v>4.1220404040404039</v>
       </c>
       <c r="C19">
         <f t="shared" ref="C19:D46" si="6">(C$2+((SUM($A19-1)/SUM($A$101-1))*(SUM(C$101-C$2))))</f>
@@ -2264,7 +2264,7 @@
       </c>
       <c r="B20">
         <f t="shared" si="5"/>
-        <v>5.5363636363636362</v>
+        <v>4.3644545454545458</v>
       </c>
       <c r="C20">
         <f t="shared" si="6"/>
@@ -2327,7 +2327,7 @@
       </c>
       <c r="B21">
         <f t="shared" si="5"/>
-        <v>5.8383838383838373</v>
+        <v>4.6068686868686868</v>
       </c>
       <c r="C21">
         <f t="shared" si="6"/>
@@ -2390,7 +2390,7 @@
       </c>
       <c r="B22">
         <f t="shared" si="5"/>
-        <v>6.1404040404040394</v>
+        <v>4.8492828282828286</v>
       </c>
       <c r="C22">
         <f t="shared" si="6"/>
@@ -2453,7 +2453,7 @@
       </c>
       <c r="B23">
         <f t="shared" si="5"/>
-        <v>6.4424242424242424</v>
+        <v>5.0916969696969696</v>
       </c>
       <c r="C23">
         <f t="shared" si="6"/>
@@ -2516,7 +2516,7 @@
       </c>
       <c r="B24">
         <f t="shared" si="5"/>
-        <v>6.7444444444444436</v>
+        <v>5.3341111111111106</v>
       </c>
       <c r="C24">
         <f t="shared" si="6"/>
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B25">
         <f t="shared" si="5"/>
-        <v>7.0464646464646457</v>
+        <v>5.5765252525252524</v>
       </c>
       <c r="C25">
         <f t="shared" si="6"/>
@@ -2642,7 +2642,7 @@
       </c>
       <c r="B26">
         <f t="shared" si="5"/>
-        <v>7.3484848484848477</v>
+        <v>5.8189393939393943</v>
       </c>
       <c r="C26">
         <f t="shared" si="6"/>
@@ -2705,7 +2705,7 @@
       </c>
       <c r="B27">
         <f t="shared" si="5"/>
-        <v>7.6505050505050507</v>
+        <v>6.0613535353535362</v>
       </c>
       <c r="C27">
         <f t="shared" si="6"/>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="B28">
         <f t="shared" si="5"/>
-        <v>7.9525252525252528</v>
+        <v>6.3037676767676771</v>
       </c>
       <c r="C28">
         <f t="shared" si="6"/>
@@ -2831,7 +2831,7 @@
       </c>
       <c r="B29">
         <f t="shared" si="5"/>
-        <v>8.254545454545454</v>
+        <v>6.5461818181818181</v>
       </c>
       <c r="C29">
         <f t="shared" si="6"/>
@@ -2894,7 +2894,7 @@
       </c>
       <c r="B30">
         <f t="shared" si="5"/>
-        <v>8.556565656565656</v>
+        <v>6.7885959595959591</v>
       </c>
       <c r="C30">
         <f t="shared" si="6"/>
@@ -2957,7 +2957,7 @@
       </c>
       <c r="B31">
         <f t="shared" si="5"/>
-        <v>8.8585858585858581</v>
+        <v>7.0310101010101009</v>
       </c>
       <c r="C31">
         <f t="shared" si="6"/>
@@ -3020,7 +3020,7 @@
       </c>
       <c r="B32">
         <f t="shared" si="5"/>
-        <v>9.1606060606060602</v>
+        <v>7.2734242424242428</v>
       </c>
       <c r="C32">
         <f t="shared" si="6"/>
@@ -3083,7 +3083,7 @@
       </c>
       <c r="B33">
         <f t="shared" si="5"/>
-        <v>9.4626262626262623</v>
+        <v>7.5158383838383847</v>
       </c>
       <c r="C33">
         <f t="shared" si="6"/>
@@ -3146,7 +3146,7 @@
       </c>
       <c r="B34">
         <f t="shared" si="5"/>
-        <v>9.7646464646464644</v>
+        <v>7.7582525252525256</v>
       </c>
       <c r="C34">
         <f t="shared" si="6"/>
@@ -3209,7 +3209,7 @@
       </c>
       <c r="B35">
         <f t="shared" si="5"/>
-        <v>10.066666666666665</v>
+        <v>8.0006666666666657</v>
       </c>
       <c r="C35">
         <f t="shared" si="6"/>
@@ -3272,7 +3272,7 @@
       </c>
       <c r="B36">
         <f t="shared" si="5"/>
-        <v>10.368686868686867</v>
+        <v>8.2430808080808067</v>
       </c>
       <c r="C36">
         <f t="shared" si="6"/>
@@ -3335,7 +3335,7 @@
       </c>
       <c r="B37">
         <f t="shared" si="5"/>
-        <v>10.670707070707071</v>
+        <v>8.4854949494949476</v>
       </c>
       <c r="C37">
         <f t="shared" si="6"/>
@@ -3398,7 +3398,7 @@
       </c>
       <c r="B38">
         <f t="shared" si="5"/>
-        <v>10.972727272727273</v>
+        <v>8.7279090909090904</v>
       </c>
       <c r="C38">
         <f t="shared" si="6"/>
@@ -3461,7 +3461,7 @@
       </c>
       <c r="B39">
         <f t="shared" si="5"/>
-        <v>11.274747474747475</v>
+        <v>8.9703232323232314</v>
       </c>
       <c r="C39">
         <f t="shared" si="6"/>
@@ -3524,7 +3524,7 @@
       </c>
       <c r="B40">
         <f t="shared" si="5"/>
-        <v>11.576767676767675</v>
+        <v>9.2127373737373723</v>
       </c>
       <c r="C40">
         <f t="shared" si="6"/>
@@ -3587,7 +3587,7 @@
       </c>
       <c r="B41">
         <f t="shared" si="5"/>
-        <v>11.878787878787877</v>
+        <v>9.4551515151515133</v>
       </c>
       <c r="C41">
         <f t="shared" si="6"/>
@@ -3650,7 +3650,7 @@
       </c>
       <c r="B42">
         <f t="shared" si="5"/>
-        <v>12.180808080808079</v>
+        <v>9.6975656565656561</v>
       </c>
       <c r="C42">
         <f t="shared" si="6"/>
@@ -3713,7 +3713,7 @@
       </c>
       <c r="B43">
         <f t="shared" si="5"/>
-        <v>12.482828282828281</v>
+        <v>9.939979797979797</v>
       </c>
       <c r="C43">
         <f t="shared" si="6"/>
@@ -3776,7 +3776,7 @@
       </c>
       <c r="B44">
         <f t="shared" si="5"/>
-        <v>12.784848484848485</v>
+        <v>10.182393939393938</v>
       </c>
       <c r="C44">
         <f t="shared" si="6"/>
@@ -3839,7 +3839,7 @@
       </c>
       <c r="B45">
         <f t="shared" si="5"/>
-        <v>13.086868686868687</v>
+        <v>10.424808080808081</v>
       </c>
       <c r="C45">
         <f t="shared" si="6"/>
@@ -3902,7 +3902,7 @@
       </c>
       <c r="B46">
         <f t="shared" si="5"/>
-        <v>13.388888888888888</v>
+        <v>10.66722222222222</v>
       </c>
       <c r="C46">
         <f t="shared" ref="C46:C77" si="11">(C$2+((SUM(A46-1)/SUM(A$101-1))*(SUM(C$101-C$2))))</f>
@@ -3965,7 +3965,7 @@
       </c>
       <c r="B47">
         <f t="shared" si="5"/>
-        <v>13.69090909090909</v>
+        <v>10.909636363636363</v>
       </c>
       <c r="C47">
         <f t="shared" si="11"/>
@@ -4028,7 +4028,7 @@
       </c>
       <c r="B48">
         <f t="shared" si="5"/>
-        <v>13.992929292929292</v>
+        <v>11.152050505050504</v>
       </c>
       <c r="C48">
         <f t="shared" si="11"/>
@@ -4091,7 +4091,7 @@
       </c>
       <c r="B49">
         <f t="shared" si="5"/>
-        <v>14.294949494949494</v>
+        <v>11.394464646464645</v>
       </c>
       <c r="C49">
         <f t="shared" si="11"/>
@@ -4154,7 +4154,7 @@
       </c>
       <c r="B50">
         <f t="shared" si="5"/>
-        <v>14.596969696969696</v>
+        <v>11.636878787878787</v>
       </c>
       <c r="C50">
         <f t="shared" si="11"/>
@@ -4217,7 +4217,7 @@
       </c>
       <c r="B51">
         <f t="shared" si="5"/>
-        <v>14.898989898989898</v>
+        <v>11.879292929292928</v>
       </c>
       <c r="C51">
         <f t="shared" si="11"/>
@@ -4280,7 +4280,7 @@
       </c>
       <c r="B52">
         <f t="shared" si="5"/>
-        <v>15.201010101010102</v>
+        <v>12.121707070707071</v>
       </c>
       <c r="C52">
         <f t="shared" si="11"/>
@@ -4343,7 +4343,7 @@
       </c>
       <c r="B53">
         <f t="shared" si="5"/>
-        <v>15.503030303030302</v>
+        <v>12.36412121212121</v>
       </c>
       <c r="C53">
         <f t="shared" si="11"/>
@@ -4406,7 +4406,7 @@
       </c>
       <c r="B54">
         <f t="shared" si="5"/>
-        <v>15.805050505050506</v>
+        <v>12.606535353535353</v>
       </c>
       <c r="C54">
         <f t="shared" si="11"/>
@@ -4469,7 +4469,7 @@
       </c>
       <c r="B55">
         <f t="shared" si="5"/>
-        <v>16.107070707070708</v>
+        <v>12.848949494949494</v>
       </c>
       <c r="C55">
         <f t="shared" si="11"/>
@@ -4532,7 +4532,7 @@
       </c>
       <c r="B56">
         <f t="shared" si="5"/>
-        <v>16.40909090909091</v>
+        <v>13.091363636363635</v>
       </c>
       <c r="C56">
         <f t="shared" si="11"/>
@@ -4595,7 +4595,7 @@
       </c>
       <c r="B57">
         <f t="shared" si="5"/>
-        <v>16.711111111111112</v>
+        <v>13.333777777777778</v>
       </c>
       <c r="C57">
         <f t="shared" si="11"/>
@@ -4658,7 +4658,7 @@
       </c>
       <c r="B58">
         <f t="shared" si="5"/>
-        <v>17.013131313131314</v>
+        <v>13.576191919191917</v>
       </c>
       <c r="C58">
         <f t="shared" si="11"/>
@@ -4721,7 +4721,7 @@
       </c>
       <c r="B59">
         <f t="shared" si="5"/>
-        <v>17.315151515151516</v>
+        <v>13.81860606060606</v>
       </c>
       <c r="C59">
         <f t="shared" si="11"/>
@@ -4784,7 +4784,7 @@
       </c>
       <c r="B60">
         <f t="shared" si="5"/>
-        <v>17.617171717171718</v>
+        <v>14.061020202020201</v>
       </c>
       <c r="C60">
         <f t="shared" si="11"/>
@@ -4847,7 +4847,7 @@
       </c>
       <c r="B61">
         <f t="shared" si="5"/>
-        <v>17.919191919191917</v>
+        <v>14.303434343434342</v>
       </c>
       <c r="C61">
         <f t="shared" si="11"/>
@@ -4910,7 +4910,7 @@
       </c>
       <c r="B62">
         <f t="shared" si="5"/>
-        <v>18.221212121212123</v>
+        <v>14.545848484848484</v>
       </c>
       <c r="C62">
         <f t="shared" si="11"/>
@@ -4973,7 +4973,7 @@
       </c>
       <c r="B63">
         <f t="shared" si="5"/>
-        <v>18.523232323232325</v>
+        <v>14.788262626262624</v>
       </c>
       <c r="C63">
         <f t="shared" si="11"/>
@@ -5036,7 +5036,7 @@
       </c>
       <c r="B64">
         <f t="shared" si="5"/>
-        <v>18.825252525252527</v>
+        <v>15.030676767676768</v>
       </c>
       <c r="C64">
         <f t="shared" si="11"/>
@@ -5099,7 +5099,7 @@
       </c>
       <c r="B65">
         <f t="shared" si="5"/>
-        <v>19.127272727272729</v>
+        <v>15.273090909090907</v>
       </c>
       <c r="C65">
         <f t="shared" si="11"/>
@@ -5162,7 +5162,7 @@
       </c>
       <c r="B66">
         <f t="shared" si="5"/>
-        <v>19.429292929292931</v>
+        <v>15.51550505050505</v>
       </c>
       <c r="C66">
         <f t="shared" si="11"/>
@@ -5225,7 +5225,7 @@
       </c>
       <c r="B67">
         <f t="shared" si="5"/>
-        <v>19.731313131313133</v>
+        <v>15.757919191919191</v>
       </c>
       <c r="C67">
         <f t="shared" si="11"/>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="B68">
         <f t="shared" ref="B68:B100" si="14">(B$2+((SUM(A68-1)/SUM(A$101-1))*(SUM(B$101-B$2))))</f>
-        <v>20.033333333333331</v>
+        <v>16.000333333333334</v>
       </c>
       <c r="C68">
         <f t="shared" si="11"/>
@@ -5351,7 +5351,7 @@
       </c>
       <c r="B69">
         <f t="shared" si="14"/>
-        <v>20.335353535353537</v>
+        <v>16.242747474747475</v>
       </c>
       <c r="C69">
         <f t="shared" si="11"/>
@@ -5414,7 +5414,7 @@
       </c>
       <c r="B70">
         <f t="shared" si="14"/>
-        <v>20.637373737373736</v>
+        <v>16.485161616161616</v>
       </c>
       <c r="C70">
         <f t="shared" si="11"/>
@@ -5477,7 +5477,7 @@
       </c>
       <c r="B71">
         <f t="shared" si="14"/>
-        <v>20.939393939393941</v>
+        <v>16.72757575757576</v>
       </c>
       <c r="C71">
         <f t="shared" si="11"/>
@@ -5540,7 +5540,7 @@
       </c>
       <c r="B72">
         <f t="shared" si="14"/>
-        <v>21.241414141414143</v>
+        <v>16.969989898989898</v>
       </c>
       <c r="C72">
         <f t="shared" si="11"/>
@@ -5603,7 +5603,7 @@
       </c>
       <c r="B73">
         <f t="shared" si="14"/>
-        <v>21.543434343434342</v>
+        <v>17.212404040404039</v>
       </c>
       <c r="C73">
         <f t="shared" si="11"/>
@@ -5666,7 +5666,7 @@
       </c>
       <c r="B74">
         <f t="shared" si="14"/>
-        <v>21.845454545454547</v>
+        <v>17.454818181818183</v>
       </c>
       <c r="C74">
         <f t="shared" si="11"/>
@@ -5729,7 +5729,7 @@
       </c>
       <c r="B75">
         <f t="shared" si="14"/>
-        <v>22.147474747474746</v>
+        <v>17.697232323232324</v>
       </c>
       <c r="C75">
         <f t="shared" si="11"/>
@@ -5792,7 +5792,7 @@
       </c>
       <c r="B76">
         <f t="shared" si="14"/>
-        <v>22.449494949494952</v>
+        <v>17.939646464646465</v>
       </c>
       <c r="C76">
         <f t="shared" si="11"/>
@@ -5855,7 +5855,7 @@
       </c>
       <c r="B77">
         <f t="shared" si="14"/>
-        <v>22.75151515151515</v>
+        <v>18.182060606060606</v>
       </c>
       <c r="C77">
         <f t="shared" si="11"/>
@@ -5918,7 +5918,7 @@
       </c>
       <c r="B78">
         <f t="shared" si="14"/>
-        <v>23.053535353535352</v>
+        <v>18.424474747474747</v>
       </c>
       <c r="C78">
         <f t="shared" ref="C78:C100" si="15">(C$2+((SUM(A78-1)/SUM(A$101-1))*(SUM(C$101-C$2))))</f>
@@ -5981,7 +5981,7 @@
       </c>
       <c r="B79">
         <f t="shared" si="14"/>
-        <v>23.355555555555558</v>
+        <v>18.666888888888888</v>
       </c>
       <c r="C79">
         <f t="shared" si="15"/>
@@ -6044,7 +6044,7 @@
       </c>
       <c r="B80">
         <f t="shared" si="14"/>
-        <v>23.657575757575756</v>
+        <v>18.909303030303029</v>
       </c>
       <c r="C80">
         <f t="shared" si="15"/>
@@ -6107,7 +6107,7 @@
       </c>
       <c r="B81">
         <f t="shared" si="14"/>
-        <v>23.959595959595962</v>
+        <v>19.151717171717173</v>
       </c>
       <c r="C81">
         <f t="shared" si="15"/>
@@ -6170,7 +6170,7 @@
       </c>
       <c r="B82">
         <f t="shared" si="14"/>
-        <v>24.261616161616161</v>
+        <v>19.394131313131314</v>
       </c>
       <c r="C82">
         <f t="shared" si="15"/>
@@ -6233,7 +6233,7 @@
       </c>
       <c r="B83">
         <f t="shared" si="14"/>
-        <v>24.563636363636366</v>
+        <v>19.636545454545455</v>
       </c>
       <c r="C83">
         <f t="shared" si="15"/>
@@ -6296,7 +6296,7 @@
       </c>
       <c r="B84">
         <f t="shared" si="14"/>
-        <v>24.865656565656565</v>
+        <v>19.878959595959596</v>
       </c>
       <c r="C84">
         <f t="shared" si="15"/>
@@ -6359,7 +6359,7 @@
       </c>
       <c r="B85">
         <f t="shared" si="14"/>
-        <v>25.167676767676767</v>
+        <v>20.121373737373737</v>
       </c>
       <c r="C85">
         <f t="shared" si="15"/>
@@ -6422,7 +6422,7 @@
       </c>
       <c r="B86">
         <f t="shared" si="14"/>
-        <v>25.469696969696972</v>
+        <v>20.363787878787878</v>
       </c>
       <c r="C86">
         <f t="shared" si="15"/>
@@ -6485,7 +6485,7 @@
       </c>
       <c r="B87">
         <f t="shared" si="14"/>
-        <v>25.771717171717171</v>
+        <v>20.606202020202019</v>
       </c>
       <c r="C87">
         <f t="shared" si="15"/>
@@ -6548,7 +6548,7 @@
       </c>
       <c r="B88">
         <f t="shared" si="14"/>
-        <v>26.073737373737377</v>
+        <v>20.848616161616164</v>
       </c>
       <c r="C88">
         <f t="shared" si="15"/>
@@ -6611,7 +6611,7 @@
       </c>
       <c r="B89">
         <f t="shared" si="14"/>
-        <v>26.375757575757575</v>
+        <v>21.091030303030305</v>
       </c>
       <c r="C89">
         <f t="shared" si="15"/>
@@ -6674,7 +6674,7 @@
       </c>
       <c r="B90">
         <f t="shared" si="14"/>
-        <v>26.677777777777777</v>
+        <v>21.333444444444442</v>
       </c>
       <c r="C90">
         <f t="shared" si="15"/>
@@ -6737,7 +6737,7 @@
       </c>
       <c r="B91">
         <f t="shared" si="14"/>
-        <v>26.979797979797979</v>
+        <v>21.575858585858587</v>
       </c>
       <c r="C91">
         <f t="shared" si="15"/>
@@ -6800,7 +6800,7 @@
       </c>
       <c r="B92">
         <f t="shared" si="14"/>
-        <v>27.281818181818181</v>
+        <v>21.818272727272728</v>
       </c>
       <c r="C92">
         <f t="shared" si="15"/>
@@ -6863,7 +6863,7 @@
       </c>
       <c r="B93">
         <f t="shared" si="14"/>
-        <v>27.583838383838383</v>
+        <v>22.060686868686869</v>
       </c>
       <c r="C93">
         <f t="shared" si="15"/>
@@ -6926,7 +6926,7 @@
       </c>
       <c r="B94">
         <f t="shared" si="14"/>
-        <v>27.885858585858585</v>
+        <v>22.30310101010101</v>
       </c>
       <c r="C94">
         <f t="shared" si="15"/>
@@ -6989,7 +6989,7 @@
       </c>
       <c r="B95">
         <f t="shared" si="14"/>
-        <v>28.187878787878791</v>
+        <v>22.545515151515154</v>
       </c>
       <c r="C95">
         <f t="shared" si="15"/>
@@ -7052,7 +7052,7 @@
       </c>
       <c r="B96">
         <f t="shared" si="14"/>
-        <v>28.48989898989899</v>
+        <v>22.787929292929292</v>
       </c>
       <c r="C96">
         <f t="shared" si="15"/>
@@ -7115,7 +7115,7 @@
       </c>
       <c r="B97">
         <f t="shared" si="14"/>
-        <v>28.791919191919192</v>
+        <v>23.030343434343433</v>
       </c>
       <c r="C97">
         <f t="shared" si="15"/>
@@ -7178,7 +7178,7 @@
       </c>
       <c r="B98">
         <f t="shared" si="14"/>
-        <v>29.093939393939394</v>
+        <v>23.272757575757577</v>
       </c>
       <c r="C98">
         <f t="shared" si="15"/>
@@ -7241,7 +7241,7 @@
       </c>
       <c r="B99">
         <f t="shared" si="14"/>
-        <v>29.395959595959596</v>
+        <v>23.515171717171718</v>
       </c>
       <c r="C99">
         <f t="shared" si="15"/>
@@ -7304,7 +7304,7 @@
       </c>
       <c r="B100">
         <f t="shared" si="14"/>
-        <v>29.697979797979798</v>
+        <v>23.757585858585859</v>
       </c>
       <c r="C100">
         <f t="shared" si="15"/>
@@ -7366,7 +7366,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="1">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C101" s="1">
         <v>0.2</v>

</xml_diff>